<commit_message>
feat: Adicionar funcionalidade de login para o município de Guarulhos
</commit_message>
<xml_diff>
--- a/ValidarAcessoPrefeituras.xlsx
+++ b/ValidarAcessoPrefeituras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ander\OneDrive\Área de Trabalho\AcessoPrefeituras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D9D4AA-7A76-4376-9C0B-55508BEC9EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C529D9CF-AA08-4C6D-A4B5-ACBFEB35FED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="160">
   <si>
     <t>Status</t>
   </si>
@@ -449,6 +449,57 @@
   </si>
   <si>
     <t>https://portal.gissonline.com.br/</t>
+  </si>
+  <si>
+    <t>NOVACASABAHIA</t>
+  </si>
+  <si>
+    <t>014575</t>
+  </si>
+  <si>
+    <t>038495</t>
+  </si>
+  <si>
+    <t>077933</t>
+  </si>
+  <si>
+    <t>077934</t>
+  </si>
+  <si>
+    <t>098886</t>
+  </si>
+  <si>
+    <t>093732</t>
+  </si>
+  <si>
+    <t>106240</t>
+  </si>
+  <si>
+    <t>208584</t>
+  </si>
+  <si>
+    <t>292044</t>
+  </si>
+  <si>
+    <t>349352</t>
+  </si>
+  <si>
+    <t>352093</t>
+  </si>
+  <si>
+    <t>via2020</t>
+  </si>
+  <si>
+    <t>w2020</t>
+  </si>
+  <si>
+    <t>208584pf</t>
+  </si>
+  <si>
+    <t>pf106240</t>
+  </si>
+  <si>
+    <t>pf93732</t>
   </si>
 </sst>
 </file>
@@ -548,7 +599,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -564,6 +615,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -871,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="K102" sqref="K102"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +945,7 @@
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="78.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -4067,6 +4123,12 @@
       <c r="K102" t="s">
         <v>142</v>
       </c>
+      <c r="L102" s="7">
+        <v>104321</v>
+      </c>
+      <c r="M102" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="103" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
@@ -4090,6 +4152,12 @@
       <c r="K103" t="s">
         <v>142</v>
       </c>
+      <c r="L103" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="M103" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="104" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
@@ -4113,6 +4181,12 @@
       <c r="K104" t="s">
         <v>142</v>
       </c>
+      <c r="L104" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="M104" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="105" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
@@ -4136,6 +4210,12 @@
       <c r="K105" t="s">
         <v>142</v>
       </c>
+      <c r="L105" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M105" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="106" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
@@ -4159,6 +4239,12 @@
       <c r="K106" t="s">
         <v>142</v>
       </c>
+      <c r="L106" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="M106" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="107" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
@@ -4182,6 +4268,12 @@
       <c r="K107" t="s">
         <v>142</v>
       </c>
+      <c r="L107" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="M107" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="108" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
@@ -4205,6 +4297,12 @@
       <c r="K108" t="s">
         <v>142</v>
       </c>
+      <c r="L108" s="7">
+        <v>106351</v>
+      </c>
+      <c r="M108" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="109" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
@@ -4228,6 +4326,12 @@
       <c r="K109" t="s">
         <v>142</v>
       </c>
+      <c r="L109" s="7">
+        <v>126415</v>
+      </c>
+      <c r="M109" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="110" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D110" t="s">
@@ -4251,6 +4355,12 @@
       <c r="K110" t="s">
         <v>142</v>
       </c>
+      <c r="L110" s="7">
+        <v>134398</v>
+      </c>
+      <c r="M110" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="111" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
@@ -4274,6 +4384,12 @@
       <c r="K111" t="s">
         <v>142</v>
       </c>
+      <c r="L111" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="M111" s="9" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="112" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
@@ -4297,8 +4413,14 @@
       <c r="K112" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="113" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L112" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="M112" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="113" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
         <v>121</v>
       </c>
@@ -4320,8 +4442,14 @@
       <c r="K113" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="114" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L113" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="M113" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="114" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
         <v>121</v>
       </c>
@@ -4343,8 +4471,14 @@
       <c r="K114" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="115" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L114" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="M114" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="115" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
         <v>121</v>
       </c>
@@ -4366,8 +4500,14 @@
       <c r="K115" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="116" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="L115" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="M115" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="116" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
         <v>121</v>
       </c>
@@ -4388,6 +4528,12 @@
       </c>
       <c r="K116" t="s">
         <v>142</v>
+      </c>
+      <c r="L116" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="M116" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add login functionality for Guarulhos municipality
</commit_message>
<xml_diff>
--- a/ValidarAcessoPrefeituras.xlsx
+++ b/ValidarAcessoPrefeituras.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="195">
   <si>
     <t>Status</t>
   </si>
@@ -115,6 +115,9 @@
     <t>Guarulhos</t>
   </si>
   <si>
+    <t>Curitiba</t>
+  </si>
+  <si>
     <t>RJ</t>
   </si>
   <si>
@@ -142,6 +145,9 @@
     <t>BA</t>
   </si>
   <si>
+    <t>PR</t>
+  </si>
+  <si>
     <t>33.041.260/1567-68</t>
   </si>
   <si>
@@ -217,6 +223,60 @@
     <t>104321-85</t>
   </si>
   <si>
+    <t>407978-8</t>
+  </si>
+  <si>
+    <t>363264-0</t>
+  </si>
+  <si>
+    <t>361029-7</t>
+  </si>
+  <si>
+    <t>408013-0</t>
+  </si>
+  <si>
+    <t>407988-2</t>
+  </si>
+  <si>
+    <t>408693-9</t>
+  </si>
+  <si>
+    <t>408058-6</t>
+  </si>
+  <si>
+    <t>0542144-1</t>
+  </si>
+  <si>
+    <t>648672-1</t>
+  </si>
+  <si>
+    <t>665812-0</t>
+  </si>
+  <si>
+    <t>665832-0</t>
+  </si>
+  <si>
+    <t>665829-0</t>
+  </si>
+  <si>
+    <t>665830-2</t>
+  </si>
+  <si>
+    <t>665813-4</t>
+  </si>
+  <si>
+    <t>665811-7</t>
+  </si>
+  <si>
+    <t>665833-3</t>
+  </si>
+  <si>
+    <t>665828-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0825503-0 </t>
+  </si>
+  <si>
     <t>RJ 3300407</t>
   </si>
   <si>
@@ -271,6 +331,9 @@
     <t>SP 3518800</t>
   </si>
   <si>
+    <t>PR 4106902</t>
+  </si>
+  <si>
     <t>TRIBUTOS</t>
   </si>
   <si>
@@ -364,6 +427,9 @@
     <t>https://portal.gissonline.com.br/</t>
   </si>
   <si>
+    <t>https://isscuritiba.curitiba.pr.gov.br/iss/default.aspx</t>
+  </si>
+  <si>
     <t>043.844.518-06</t>
   </si>
   <si>
@@ -470,6 +536,45 @@
   </si>
   <si>
     <t>via2020</t>
+  </si>
+  <si>
+    <t>036754</t>
+  </si>
+  <si>
+    <t>@vv2020o</t>
+  </si>
+  <si>
+    <t>Fiscal135</t>
+  </si>
+  <si>
+    <t>@Fiscal135</t>
+  </si>
+  <si>
+    <t>FISCAL206</t>
+  </si>
+  <si>
+    <t>VIA2022</t>
+  </si>
+  <si>
+    <t>Via2023#</t>
+  </si>
+  <si>
+    <t>via2024@</t>
+  </si>
+  <si>
+    <t>Via2022*</t>
+  </si>
+  <si>
+    <t>via2023@</t>
+  </si>
+  <si>
+    <t>via22*</t>
+  </si>
+  <si>
+    <t>VAREJO21*</t>
+  </si>
+  <si>
+    <t>Via2023!</t>
   </si>
   <si>
     <t>SIM</t>
@@ -864,7 +969,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O116"/>
+  <dimension ref="A1:O136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -925,7 +1030,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <v>33041260079089</v>
@@ -937,22 +1042,22 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="L2" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="M2" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="O2" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -963,7 +1068,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3">
         <v>33041260113791</v>
@@ -975,13 +1080,13 @@
         <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="L3">
         <v>33041260113791</v>
@@ -990,7 +1095,7 @@
         <v>33041260</v>
       </c>
       <c r="O3" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1001,10 +1106,10 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G4">
         <v>27331</v>
@@ -1013,25 +1118,25 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="L4">
         <v>33041260156768</v>
       </c>
       <c r="M4" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="N4" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="O4" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1042,10 +1147,10 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>1355030014</v>
@@ -1054,25 +1159,25 @@
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="L5">
         <v>33041260134799</v>
       </c>
       <c r="M5" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="N5" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="O5" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1083,7 +1188,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F6">
         <v>33041260109255</v>
@@ -1095,22 +1200,22 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="J6" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="L6" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="M6" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="O6" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1121,7 +1226,7 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7">
         <v>33041260129523</v>
@@ -1133,22 +1238,22 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="J7" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="L7">
         <v>33041260129523</v>
       </c>
       <c r="M7" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="O7" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1159,7 +1264,7 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8">
         <v>33041260028093</v>
@@ -1171,22 +1276,22 @@
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J8" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="L8" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="N8" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="O8" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1197,7 +1302,7 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9">
         <v>33041260020947</v>
@@ -1209,22 +1314,22 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J9" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="L9" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="N9" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="O9" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1235,7 +1340,7 @@
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10">
         <v>33041260030829</v>
@@ -1247,22 +1352,22 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J10" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="L10" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="N10" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="O10" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1273,7 +1378,7 @@
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11">
         <v>33041260069954</v>
@@ -1285,22 +1390,22 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J11" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="L11" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="N11" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="O11" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1311,7 +1416,7 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12">
         <v>33041260171805</v>
@@ -1323,22 +1428,22 @@
         <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="J12" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="L12" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="M12" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="O12" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1349,7 +1454,7 @@
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13">
         <v>33041260151960</v>
@@ -1361,13 +1466,13 @@
         <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="J13" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="L13">
         <v>33041260151960</v>
@@ -1376,7 +1481,7 @@
         <v>783856</v>
       </c>
       <c r="O13" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1387,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14">
         <v>33041260177170</v>
@@ -1399,22 +1504,22 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="J14" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="L14" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="M14" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="O14" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1425,7 +1530,7 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15">
         <v>33041260109921</v>
@@ -1437,25 +1542,25 @@
         <v>20</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="J15" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="L15">
         <v>33041260109921</v>
       </c>
       <c r="M15" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="N15" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="O15" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1466,7 +1571,7 @@
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16">
         <v>33041260193027</v>
@@ -1478,22 +1583,22 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="J16" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="L16">
         <v>33041260193027</v>
       </c>
       <c r="M16" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="O16" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="3:15">
@@ -1504,7 +1609,7 @@
         <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>33041260194503</v>
@@ -1516,22 +1621,22 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="J17" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="L17" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="M17" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="O17" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="3:15">
@@ -1542,10 +1647,10 @@
         <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G18">
         <v>14969</v>
@@ -1554,25 +1659,25 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J18" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="L18" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="M18" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="N18" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="O18" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="3:15">
@@ -1583,10 +1688,10 @@
         <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G19">
         <v>16999</v>
@@ -1595,25 +1700,25 @@
         <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="J19" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="L19">
         <v>25856654889</v>
       </c>
       <c r="M19" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="N19" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="O19" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="3:15">
@@ -1624,7 +1729,7 @@
         <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20">
         <v>33041260127407</v>
@@ -1636,13 +1741,13 @@
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="J20" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="L20">
         <v>33041260127407</v>
@@ -1651,7 +1756,7 @@
         <v>1033</v>
       </c>
       <c r="O20" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="3:15">
@@ -1659,7 +1764,7 @@
         <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F21">
         <v>33041260032953</v>
@@ -1671,19 +1776,19 @@
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L21" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M21" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O21" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="3:15">
@@ -1691,7 +1796,7 @@
         <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F22">
         <v>33041260001489</v>
@@ -1703,19 +1808,19 @@
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L22" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M22" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O22" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="3:15">
@@ -1723,7 +1828,7 @@
         <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F23">
         <v>33041260005042</v>
@@ -1735,19 +1840,19 @@
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L23" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M23" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O23" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="3:15">
@@ -1755,7 +1860,7 @@
         <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F24">
         <v>33041260009463</v>
@@ -1767,19 +1872,19 @@
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L24" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M24" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O24" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="3:15">
@@ -1787,7 +1892,7 @@
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F25">
         <v>33041260002965</v>
@@ -1799,19 +1904,19 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L25" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M25" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O25" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="3:15">
@@ -1819,7 +1924,7 @@
         <v>31</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F26">
         <v>33041260007339</v>
@@ -1831,19 +1936,19 @@
         <v>3</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L26" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M26" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O26" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="3:15">
@@ -1851,7 +1956,7 @@
         <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F27">
         <v>33041260000679</v>
@@ -1863,19 +1968,19 @@
         <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L27" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M27" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O27" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="3:15">
@@ -1883,7 +1988,7 @@
         <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F28">
         <v>33041260000750</v>
@@ -1895,19 +2000,19 @@
         <v>3</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L28" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M28" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O28" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="3:15">
@@ -1915,7 +2020,7 @@
         <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F29">
         <v>33041260007843</v>
@@ -1927,19 +2032,19 @@
         <v>3</v>
       </c>
       <c r="I29" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L29" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M29" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O29" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="3:15">
@@ -1947,7 +2052,7 @@
         <v>31</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F30">
         <v>33041260003007</v>
@@ -1959,19 +2064,19 @@
         <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L30" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M30" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O30" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="3:15">
@@ -1979,7 +2084,7 @@
         <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F31">
         <v>33041260003856</v>
@@ -1991,19 +2096,19 @@
         <v>3</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L31" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M31" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O31" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="3:15">
@@ -2011,7 +2116,7 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F32">
         <v>33041260011018</v>
@@ -2023,19 +2128,19 @@
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L32" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M32" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O32" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="4:15">
@@ -2043,7 +2148,7 @@
         <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F33">
         <v>33041260004747</v>
@@ -2055,19 +2160,19 @@
         <v>3</v>
       </c>
       <c r="I33" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L33" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M33" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O33" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="4:15">
@@ -2075,7 +2180,7 @@
         <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F34">
         <v>33041260004313</v>
@@ -2087,19 +2192,19 @@
         <v>3</v>
       </c>
       <c r="I34" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L34" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M34" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O34" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="4:15">
@@ -2107,7 +2212,7 @@
         <v>31</v>
       </c>
       <c r="E35" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F35">
         <v>33041260014890</v>
@@ -2119,19 +2224,19 @@
         <v>3</v>
       </c>
       <c r="I35" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L35" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M35" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O35" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="4:15">
@@ -2139,7 +2244,7 @@
         <v>31</v>
       </c>
       <c r="E36" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F36">
         <v>33041260018969</v>
@@ -2151,19 +2256,19 @@
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L36" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M36" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O36" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="4:15">
@@ -2171,7 +2276,7 @@
         <v>31</v>
       </c>
       <c r="E37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F37">
         <v>33041260034735</v>
@@ -2183,19 +2288,19 @@
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L37" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M37" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O37" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="4:15">
@@ -2203,7 +2308,7 @@
         <v>31</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F38">
         <v>33041260019264</v>
@@ -2215,19 +2320,19 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L38" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M38" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O38" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="4:15">
@@ -2235,7 +2340,7 @@
         <v>31</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F39">
         <v>33041260018020</v>
@@ -2247,19 +2352,19 @@
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L39" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M39" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O39" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="4:15">
@@ -2267,7 +2372,7 @@
         <v>31</v>
       </c>
       <c r="E40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F40">
         <v>33041260020190</v>
@@ -2279,19 +2384,19 @@
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L40" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M40" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O40" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="4:15">
@@ -2299,7 +2404,7 @@
         <v>31</v>
       </c>
       <c r="E41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F41">
         <v>33041260001560</v>
@@ -2311,19 +2416,19 @@
         <v>3</v>
       </c>
       <c r="I41" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L41" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M41" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O41" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="4:15">
@@ -2331,7 +2436,7 @@
         <v>31</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F42">
         <v>33041260048108</v>
@@ -2343,19 +2448,19 @@
         <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L42" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M42" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O42" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="4:15">
@@ -2363,7 +2468,7 @@
         <v>31</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F43">
         <v>33041260006529</v>
@@ -2375,19 +2480,19 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L43" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M43" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O43" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="4:15">
@@ -2395,7 +2500,7 @@
         <v>31</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F44">
         <v>33041260049252</v>
@@ -2407,19 +2512,19 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L44" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M44" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O44" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="4:15">
@@ -2427,7 +2532,7 @@
         <v>31</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F45">
         <v>33041260052717</v>
@@ -2439,19 +2544,19 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L45" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M45" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O45" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="4:15">
@@ -2459,7 +2564,7 @@
         <v>31</v>
       </c>
       <c r="E46" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F46">
         <v>33041260054337</v>
@@ -2471,19 +2576,19 @@
         <v>3</v>
       </c>
       <c r="I46" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L46" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M46" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O46" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="4:15">
@@ -2491,7 +2596,7 @@
         <v>31</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F47">
         <v>33041260053284</v>
@@ -2503,19 +2608,19 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L47" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M47" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O47" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="4:15">
@@ -2523,7 +2628,7 @@
         <v>31</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F48">
         <v>33041260066009</v>
@@ -2535,19 +2640,19 @@
         <v>3</v>
       </c>
       <c r="I48" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L48" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M48" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O48" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="4:15">
@@ -2555,7 +2660,7 @@
         <v>31</v>
       </c>
       <c r="E49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F49">
         <v>33041260074362</v>
@@ -2567,19 +2672,19 @@
         <v>3</v>
       </c>
       <c r="I49" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L49" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M49" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O49" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="4:15">
@@ -2587,7 +2692,7 @@
         <v>31</v>
       </c>
       <c r="E50" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F50">
         <v>33041260075849</v>
@@ -2599,19 +2704,19 @@
         <v>3</v>
       </c>
       <c r="I50" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L50" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M50" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O50" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="4:15">
@@ -2619,7 +2724,7 @@
         <v>31</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F51">
         <v>33041260077388</v>
@@ -2631,19 +2736,19 @@
         <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L51" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M51" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O51" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="4:15">
@@ -2651,7 +2756,7 @@
         <v>31</v>
       </c>
       <c r="E52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F52">
         <v>33041260147696</v>
@@ -2663,19 +2768,19 @@
         <v>3</v>
       </c>
       <c r="I52" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L52" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M52" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O52" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="4:15">
@@ -2683,7 +2788,7 @@
         <v>31</v>
       </c>
       <c r="E53" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F53">
         <v>33041260153238</v>
@@ -2695,19 +2800,19 @@
         <v>3</v>
       </c>
       <c r="I53" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L53" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M53" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O53" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="4:15">
@@ -2715,7 +2820,7 @@
         <v>31</v>
       </c>
       <c r="E54" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F54">
         <v>33041260082896</v>
@@ -2727,19 +2832,19 @@
         <v>3</v>
       </c>
       <c r="I54" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L54" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M54" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O54" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="4:15">
@@ -2747,7 +2852,7 @@
         <v>31</v>
       </c>
       <c r="E55" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F55">
         <v>33041260082977</v>
@@ -2759,19 +2864,19 @@
         <v>3</v>
       </c>
       <c r="I55" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L55" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M55" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O55" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="4:15">
@@ -2779,7 +2884,7 @@
         <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F56">
         <v>33041260083000</v>
@@ -2791,19 +2896,19 @@
         <v>3</v>
       </c>
       <c r="I56" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L56" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M56" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O56" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="4:15">
@@ -2811,7 +2916,7 @@
         <v>31</v>
       </c>
       <c r="E57" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F57">
         <v>33041260083191</v>
@@ -2823,19 +2928,19 @@
         <v>3</v>
       </c>
       <c r="I57" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L57" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M57" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O57" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="4:15">
@@ -2843,7 +2948,7 @@
         <v>31</v>
       </c>
       <c r="E58" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F58">
         <v>33041260083272</v>
@@ -2855,19 +2960,19 @@
         <v>3</v>
       </c>
       <c r="I58" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L58" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M58" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O58" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="4:15">
@@ -2875,7 +2980,7 @@
         <v>31</v>
       </c>
       <c r="E59" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F59">
         <v>33041260083353</v>
@@ -2887,19 +2992,19 @@
         <v>3</v>
       </c>
       <c r="I59" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L59" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M59" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O59" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="4:15">
@@ -2907,7 +3012,7 @@
         <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F60">
         <v>33041260083434</v>
@@ -2919,19 +3024,19 @@
         <v>3</v>
       </c>
       <c r="I60" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L60" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M60" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O60" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="4:15">
@@ -2939,7 +3044,7 @@
         <v>31</v>
       </c>
       <c r="E61" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F61">
         <v>33041260083515</v>
@@ -2951,19 +3056,19 @@
         <v>3</v>
       </c>
       <c r="I61" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L61" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M61" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O61" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="4:15">
@@ -2971,7 +3076,7 @@
         <v>31</v>
       </c>
       <c r="E62" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F62">
         <v>33041260083604</v>
@@ -2983,19 +3088,19 @@
         <v>3</v>
       </c>
       <c r="I62" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L62" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M62" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O62" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="4:15">
@@ -3003,7 +3108,7 @@
         <v>31</v>
       </c>
       <c r="E63" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F63">
         <v>33041260083787</v>
@@ -3015,19 +3120,19 @@
         <v>3</v>
       </c>
       <c r="I63" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L63" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M63" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O63" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" spans="4:15">
@@ -3035,7 +3140,7 @@
         <v>31</v>
       </c>
       <c r="E64" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F64">
         <v>33041260083868</v>
@@ -3047,19 +3152,19 @@
         <v>3</v>
       </c>
       <c r="I64" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L64" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M64" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O64" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="4:15">
@@ -3067,7 +3172,7 @@
         <v>31</v>
       </c>
       <c r="E65" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F65">
         <v>33041260083949</v>
@@ -3079,19 +3184,19 @@
         <v>3</v>
       </c>
       <c r="I65" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L65" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M65" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O65" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" spans="4:15">
@@ -3099,7 +3204,7 @@
         <v>31</v>
       </c>
       <c r="E66" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F66">
         <v>33041260084082</v>
@@ -3111,19 +3216,19 @@
         <v>3</v>
       </c>
       <c r="I66" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L66" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M66" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O66" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="4:15">
@@ -3131,7 +3236,7 @@
         <v>31</v>
       </c>
       <c r="E67" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F67">
         <v>33041260084163</v>
@@ -3143,19 +3248,19 @@
         <v>3</v>
       </c>
       <c r="I67" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L67" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M67" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O67" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="4:15">
@@ -3163,7 +3268,7 @@
         <v>31</v>
       </c>
       <c r="E68" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F68">
         <v>33041260084244</v>
@@ -3175,19 +3280,19 @@
         <v>3</v>
       </c>
       <c r="I68" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L68" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M68" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O68" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="4:15">
@@ -3195,7 +3300,7 @@
         <v>31</v>
       </c>
       <c r="E69" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F69">
         <v>33041260084325</v>
@@ -3207,19 +3312,19 @@
         <v>3</v>
       </c>
       <c r="I69" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L69" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M69" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O69" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="4:15">
@@ -3227,7 +3332,7 @@
         <v>31</v>
       </c>
       <c r="E70" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F70">
         <v>33041260084406</v>
@@ -3239,19 +3344,19 @@
         <v>3</v>
       </c>
       <c r="I70" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L70" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M70" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O70" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="4:15">
@@ -3259,7 +3364,7 @@
         <v>31</v>
       </c>
       <c r="E71" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F71">
         <v>33041260084678</v>
@@ -3271,19 +3376,19 @@
         <v>3</v>
       </c>
       <c r="I71" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L71" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M71" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O71" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="4:15">
@@ -3291,7 +3396,7 @@
         <v>31</v>
       </c>
       <c r="E72" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F72">
         <v>33041260084759</v>
@@ -3303,19 +3408,19 @@
         <v>3</v>
       </c>
       <c r="I72" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L72" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M72" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O72" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="4:15">
@@ -3323,7 +3428,7 @@
         <v>31</v>
       </c>
       <c r="E73" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F73">
         <v>33041260084830</v>
@@ -3335,19 +3440,19 @@
         <v>3</v>
       </c>
       <c r="I73" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L73" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M73" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O73" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="4:15">
@@ -3355,7 +3460,7 @@
         <v>31</v>
       </c>
       <c r="E74" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F74">
         <v>33041260084910</v>
@@ -3367,19 +3472,19 @@
         <v>3</v>
       </c>
       <c r="I74" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L74" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M74" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O74" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="4:15">
@@ -3387,7 +3492,7 @@
         <v>31</v>
       </c>
       <c r="E75" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F75">
         <v>33041260085054</v>
@@ -3399,19 +3504,19 @@
         <v>3</v>
       </c>
       <c r="I75" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L75" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M75" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O75" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="4:15">
@@ -3419,7 +3524,7 @@
         <v>31</v>
       </c>
       <c r="E76" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F76">
         <v>33041260085216</v>
@@ -3431,19 +3536,19 @@
         <v>3</v>
       </c>
       <c r="I76" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L76" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M76" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O76" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="4:15">
@@ -3451,7 +3556,7 @@
         <v>31</v>
       </c>
       <c r="E77" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F77">
         <v>33041260085305</v>
@@ -3463,19 +3568,19 @@
         <v>3</v>
       </c>
       <c r="I77" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L77" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M77" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O77" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" spans="4:15">
@@ -3483,7 +3588,7 @@
         <v>31</v>
       </c>
       <c r="E78" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F78">
         <v>33041260085488</v>
@@ -3495,19 +3600,19 @@
         <v>3</v>
       </c>
       <c r="I78" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L78" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M78" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O78" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79" spans="4:15">
@@ -3515,7 +3620,7 @@
         <v>31</v>
       </c>
       <c r="E79" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F79">
         <v>33041260085569</v>
@@ -3527,19 +3632,19 @@
         <v>3</v>
       </c>
       <c r="I79" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L79" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M79" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O79" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="4:15">
@@ -3547,7 +3652,7 @@
         <v>31</v>
       </c>
       <c r="E80" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F80">
         <v>33041260085992</v>
@@ -3559,19 +3664,19 @@
         <v>3</v>
       </c>
       <c r="I80" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L80" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M80" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O80" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="81" spans="4:15">
@@ -3579,7 +3684,7 @@
         <v>31</v>
       </c>
       <c r="E81" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F81">
         <v>33041260086026</v>
@@ -3591,19 +3696,19 @@
         <v>3</v>
       </c>
       <c r="I81" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L81" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M81" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O81" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="4:15">
@@ -3611,7 +3716,7 @@
         <v>31</v>
       </c>
       <c r="E82" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F82">
         <v>33041260086298</v>
@@ -3623,19 +3728,19 @@
         <v>3</v>
       </c>
       <c r="I82" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L82" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M82" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O82" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" spans="4:15">
@@ -3643,7 +3748,7 @@
         <v>31</v>
       </c>
       <c r="E83" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F83">
         <v>33041260086450</v>
@@ -3655,19 +3760,19 @@
         <v>3</v>
       </c>
       <c r="I83" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L83" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M83" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O83" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="84" spans="4:15">
@@ -3675,7 +3780,7 @@
         <v>31</v>
       </c>
       <c r="E84" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F84">
         <v>33041260086530</v>
@@ -3687,19 +3792,19 @@
         <v>3</v>
       </c>
       <c r="I84" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L84" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M84" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O84" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="85" spans="4:15">
@@ -3707,7 +3812,7 @@
         <v>31</v>
       </c>
       <c r="E85" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F85">
         <v>33041260086611</v>
@@ -3719,19 +3824,19 @@
         <v>3</v>
       </c>
       <c r="I85" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L85" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M85" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O85" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="86" spans="4:15">
@@ -3739,7 +3844,7 @@
         <v>31</v>
       </c>
       <c r="E86" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F86">
         <v>33041260086700</v>
@@ -3751,19 +3856,19 @@
         <v>3</v>
       </c>
       <c r="I86" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L86" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M86" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O86" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="87" spans="4:15">
@@ -3771,7 +3876,7 @@
         <v>31</v>
       </c>
       <c r="E87" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F87">
         <v>33041260086964</v>
@@ -3783,19 +3888,19 @@
         <v>3</v>
       </c>
       <c r="I87" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L87" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M87" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O87" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88" spans="4:15">
@@ -3803,7 +3908,7 @@
         <v>31</v>
       </c>
       <c r="E88" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F88">
         <v>33041260105004</v>
@@ -3815,19 +3920,19 @@
         <v>3</v>
       </c>
       <c r="I88" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L88" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M88" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O88" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="89" spans="4:15">
@@ -3835,7 +3940,7 @@
         <v>31</v>
       </c>
       <c r="E89" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F89">
         <v>33041260087006</v>
@@ -3847,19 +3952,19 @@
         <v>3</v>
       </c>
       <c r="I89" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L89" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M89" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O89" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="4:15">
@@ -3867,7 +3972,7 @@
         <v>31</v>
       </c>
       <c r="E90" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F90">
         <v>33041260104881</v>
@@ -3879,19 +3984,19 @@
         <v>3</v>
       </c>
       <c r="I90" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L90" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M90" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O90" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="91" spans="4:15">
@@ -3899,7 +4004,7 @@
         <v>31</v>
       </c>
       <c r="E91" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F91">
         <v>33041260087260</v>
@@ -3911,19 +4016,19 @@
         <v>3</v>
       </c>
       <c r="I91" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L91" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M91" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O91" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="92" spans="4:15">
@@ -3931,7 +4036,7 @@
         <v>31</v>
       </c>
       <c r="E92" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F92">
         <v>33041260121387</v>
@@ -3943,19 +4048,19 @@
         <v>3</v>
       </c>
       <c r="I92" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L92" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M92" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O92" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="93" spans="4:15">
@@ -3963,7 +4068,7 @@
         <v>31</v>
       </c>
       <c r="E93" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F93">
         <v>33041260121204</v>
@@ -3975,19 +4080,19 @@
         <v>3</v>
       </c>
       <c r="I93" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L93" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M93" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O93" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="4:15">
@@ -3995,7 +4100,7 @@
         <v>31</v>
       </c>
       <c r="E94" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F94">
         <v>33041260147424</v>
@@ -4007,19 +4112,19 @@
         <v>3</v>
       </c>
       <c r="I94" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L94" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M94" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O94" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="95" spans="4:15">
@@ -4027,7 +4132,7 @@
         <v>31</v>
       </c>
       <c r="E95" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F95">
         <v>33041260144751</v>
@@ -4039,19 +4144,19 @@
         <v>3</v>
       </c>
       <c r="I95" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L95" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M95" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O95" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="96" spans="4:15">
@@ -4059,31 +4164,31 @@
         <v>31</v>
       </c>
       <c r="E96" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F96">
         <v>33041260144166</v>
       </c>
       <c r="G96" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H96">
         <v>3</v>
       </c>
       <c r="I96" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L96" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M96" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O96" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="97" spans="4:15">
@@ -4091,7 +4196,7 @@
         <v>31</v>
       </c>
       <c r="E97" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F97">
         <v>33041260087340</v>
@@ -4103,19 +4208,19 @@
         <v>3</v>
       </c>
       <c r="I97" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L97" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M97" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O97" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="4:15">
@@ -4123,7 +4228,7 @@
         <v>31</v>
       </c>
       <c r="E98" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F98">
         <v>33041260161923</v>
@@ -4135,19 +4240,19 @@
         <v>3</v>
       </c>
       <c r="I98" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L98" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M98" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O98" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="4:15">
@@ -4155,7 +4260,7 @@
         <v>31</v>
       </c>
       <c r="E99" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F99">
         <v>33041260004070</v>
@@ -4167,19 +4272,19 @@
         <v>3</v>
       </c>
       <c r="I99" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L99" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M99" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O99" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="100" spans="4:15">
@@ -4187,31 +4292,31 @@
         <v>31</v>
       </c>
       <c r="E100" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F100">
         <v>33041260207699</v>
       </c>
       <c r="G100" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H100">
         <v>3</v>
       </c>
       <c r="I100" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L100" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M100" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O100" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="101" spans="4:15">
@@ -4219,7 +4324,7 @@
         <v>31</v>
       </c>
       <c r="E101" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F101">
         <v>33041260170167</v>
@@ -4231,19 +4336,19 @@
         <v>3</v>
       </c>
       <c r="I101" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="L101" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="M101" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="O101" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="102" spans="4:15">
@@ -4251,31 +4356,31 @@
         <v>32</v>
       </c>
       <c r="E102" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F102" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G102" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H102">
         <v>12</v>
       </c>
       <c r="I102" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L102">
         <v>104321</v>
       </c>
       <c r="M102" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O102" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="4:15">
@@ -4283,10 +4388,10 @@
         <v>32</v>
       </c>
       <c r="E103" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F103" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G103">
         <v>93732</v>
@@ -4295,19 +4400,19 @@
         <v>12</v>
       </c>
       <c r="I103" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L103" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="M103" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O103" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="4:15">
@@ -4315,10 +4420,10 @@
         <v>32</v>
       </c>
       <c r="E104" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F104" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G104">
         <v>106351</v>
@@ -4327,19 +4432,19 @@
         <v>12</v>
       </c>
       <c r="I104" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L104" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="M104" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O104" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="4:15">
@@ -4347,10 +4452,10 @@
         <v>32</v>
       </c>
       <c r="E105" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F105" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G105">
         <v>134398</v>
@@ -4359,19 +4464,19 @@
         <v>12</v>
       </c>
       <c r="I105" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L105" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="M105" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O105" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="106" spans="4:15">
@@ -4379,10 +4484,10 @@
         <v>32</v>
       </c>
       <c r="E106" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F106" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G106">
         <v>208584</v>
@@ -4391,19 +4496,19 @@
         <v>12</v>
       </c>
       <c r="I106" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L106" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="M106" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O106" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="4:15">
@@ -4411,10 +4516,10 @@
         <v>32</v>
       </c>
       <c r="E107" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F107" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G107">
         <v>292044</v>
@@ -4423,19 +4528,19 @@
         <v>12</v>
       </c>
       <c r="I107" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L107" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="M107" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O107" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="4:15">
@@ -4443,10 +4548,10 @@
         <v>32</v>
       </c>
       <c r="E108" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F108" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G108">
         <v>349352</v>
@@ -4455,19 +4560,19 @@
         <v>12</v>
       </c>
       <c r="I108" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L108">
         <v>106351</v>
       </c>
       <c r="M108" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O108" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="109" spans="4:15">
@@ -4475,10 +4580,10 @@
         <v>32</v>
       </c>
       <c r="E109" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F109" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G109">
         <v>352093</v>
@@ -4487,19 +4592,19 @@
         <v>12</v>
       </c>
       <c r="I109" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L109">
         <v>126415</v>
       </c>
       <c r="M109" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O109" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="110" spans="4:15">
@@ -4507,31 +4612,31 @@
         <v>32</v>
       </c>
       <c r="E110" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F110" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G110" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H110">
         <v>12</v>
       </c>
       <c r="I110" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L110">
         <v>134398</v>
       </c>
       <c r="M110" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O110" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" spans="4:15">
@@ -4539,31 +4644,31 @@
         <v>32</v>
       </c>
       <c r="E111" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F111" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G111" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H111">
         <v>12</v>
       </c>
       <c r="I111" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L111" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="M111" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="O111" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" spans="4:15">
@@ -4571,10 +4676,10 @@
         <v>32</v>
       </c>
       <c r="E112" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F112" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G112">
         <v>77934</v>
@@ -4583,19 +4688,19 @@
         <v>12</v>
       </c>
       <c r="I112" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L112" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="M112" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="O112" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="113" spans="4:15">
@@ -4603,10 +4708,10 @@
         <v>32</v>
       </c>
       <c r="E113" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F113" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G113">
         <v>98886</v>
@@ -4615,19 +4720,19 @@
         <v>12</v>
       </c>
       <c r="I113" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K113" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L113" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="M113" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="O113" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="114" spans="4:15">
@@ -4635,31 +4740,31 @@
         <v>32</v>
       </c>
       <c r="E114" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F114" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G114" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H114">
         <v>12</v>
       </c>
       <c r="I114" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K114" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L114" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="M114" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="O114" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="115" spans="4:15">
@@ -4667,10 +4772,10 @@
         <v>32</v>
       </c>
       <c r="E115" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F115" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G115">
         <v>106240</v>
@@ -4679,19 +4784,19 @@
         <v>12</v>
       </c>
       <c r="I115" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="L115" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="M115" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="O115" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="116" spans="4:15">
@@ -4699,10 +4804,10 @@
         <v>32</v>
       </c>
       <c r="E116" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F116" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G116">
         <v>126415</v>
@@ -4711,19 +4816,659 @@
         <v>12</v>
       </c>
       <c r="I116" t="s">
+        <v>104</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="L116" t="s">
+        <v>156</v>
+      </c>
+      <c r="M116" t="s">
+        <v>163</v>
+      </c>
+      <c r="O116" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="117" spans="4:15">
+      <c r="D117" t="s">
+        <v>33</v>
+      </c>
+      <c r="E117" t="s">
+        <v>43</v>
+      </c>
+      <c r="F117">
+        <v>33041260041197</v>
+      </c>
+      <c r="G117" t="s">
+        <v>69</v>
+      </c>
+      <c r="H117">
+        <v>20</v>
+      </c>
+      <c r="I117" t="s">
+        <v>105</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L117">
+        <v>500200</v>
+      </c>
+      <c r="M117" t="s">
+        <v>174</v>
+      </c>
+      <c r="O117" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="118" spans="4:15">
+      <c r="D118" t="s">
+        <v>33</v>
+      </c>
+      <c r="E118" t="s">
+        <v>43</v>
+      </c>
+      <c r="F118">
+        <v>33041260025159</v>
+      </c>
+      <c r="G118" t="s">
+        <v>70</v>
+      </c>
+      <c r="H118">
+        <v>20</v>
+      </c>
+      <c r="I118" t="s">
+        <v>105</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L118">
+        <v>150230</v>
+      </c>
+      <c r="M118" t="s">
+        <v>175</v>
+      </c>
+      <c r="O118" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="119" spans="4:15">
+      <c r="D119" t="s">
+        <v>33</v>
+      </c>
+      <c r="E119" t="s">
+        <v>43</v>
+      </c>
+      <c r="F119">
+        <v>33041260025310</v>
+      </c>
+      <c r="G119" t="s">
+        <v>71</v>
+      </c>
+      <c r="H119">
+        <v>20</v>
+      </c>
+      <c r="I119" t="s">
+        <v>105</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L119">
+        <v>740220</v>
+      </c>
+      <c r="M119" t="s">
+        <v>176</v>
+      </c>
+      <c r="O119" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="120" spans="4:15">
+      <c r="D120" t="s">
+        <v>33</v>
+      </c>
+      <c r="E120" t="s">
+        <v>43</v>
+      </c>
+      <c r="F120">
+        <v>33041260040204</v>
+      </c>
+      <c r="G120" t="s">
+        <v>72</v>
+      </c>
+      <c r="H120">
+        <v>20</v>
+      </c>
+      <c r="I120" t="s">
+        <v>105</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L120">
+        <v>123392</v>
+      </c>
+      <c r="M120" t="s">
+        <v>177</v>
+      </c>
+      <c r="O120" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="121" spans="4:15">
+      <c r="D121" t="s">
+        <v>33</v>
+      </c>
+      <c r="E121" t="s">
+        <v>43</v>
+      </c>
+      <c r="F121">
+        <v>33041260041278</v>
+      </c>
+      <c r="G121" t="s">
+        <v>73</v>
+      </c>
+      <c r="H121">
+        <v>20</v>
+      </c>
+      <c r="I121" t="s">
+        <v>105</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L121">
+        <v>193237</v>
+      </c>
+      <c r="M121" t="s">
+        <v>161</v>
+      </c>
+      <c r="O121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="4:15">
+      <c r="D122" t="s">
+        <v>33</v>
+      </c>
+      <c r="E122" t="s">
+        <v>43</v>
+      </c>
+      <c r="F122">
+        <v>33041260041510</v>
+      </c>
+      <c r="G122" t="s">
+        <v>74</v>
+      </c>
+      <c r="H122">
+        <v>20</v>
+      </c>
+      <c r="I122" t="s">
+        <v>105</v>
+      </c>
+      <c r="K122" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L122">
+        <v>172181</v>
+      </c>
+      <c r="M122" t="s">
+        <v>178</v>
+      </c>
+      <c r="O122" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="123" spans="4:15">
+      <c r="D123" t="s">
+        <v>33</v>
+      </c>
+      <c r="E123" t="s">
+        <v>43</v>
+      </c>
+      <c r="F123">
+        <v>33041260040387</v>
+      </c>
+      <c r="G123" t="s">
+        <v>75</v>
+      </c>
+      <c r="H123">
+        <v>20</v>
+      </c>
+      <c r="I123" t="s">
+        <v>105</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L123">
+        <v>149207</v>
+      </c>
+      <c r="M123" t="s">
+        <v>161</v>
+      </c>
+      <c r="O123" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="124" spans="4:15">
+      <c r="D124" t="s">
+        <v>33</v>
+      </c>
+      <c r="E124" t="s">
+        <v>43</v>
+      </c>
+      <c r="F124">
+        <v>33041260063832</v>
+      </c>
+      <c r="G124" t="s">
+        <v>76</v>
+      </c>
+      <c r="H124">
+        <v>20</v>
+      </c>
+      <c r="I124" t="s">
+        <v>105</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L124">
+        <v>402622</v>
+      </c>
+      <c r="M124" t="s">
+        <v>179</v>
+      </c>
+      <c r="O124" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="125" spans="4:15">
+      <c r="D125" t="s">
+        <v>33</v>
+      </c>
+      <c r="E125" t="s">
+        <v>43</v>
+      </c>
+      <c r="F125">
+        <v>33041260091020</v>
+      </c>
+      <c r="G125" t="s">
+        <v>77</v>
+      </c>
+      <c r="H125">
+        <v>20</v>
+      </c>
+      <c r="I125" t="s">
+        <v>105</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L125">
+        <v>33041260091020</v>
+      </c>
+      <c r="M125" t="s">
+        <v>180</v>
+      </c>
+      <c r="O125" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="126" spans="4:15">
+      <c r="D126" t="s">
+        <v>33</v>
+      </c>
+      <c r="E126" t="s">
+        <v>43</v>
+      </c>
+      <c r="F126">
+        <v>33041260091100</v>
+      </c>
+      <c r="G126" t="s">
+        <v>78</v>
+      </c>
+      <c r="H126">
+        <v>20</v>
+      </c>
+      <c r="I126" t="s">
+        <v>105</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L126">
+        <v>33041260091100</v>
+      </c>
+      <c r="M126" t="s">
+        <v>181</v>
+      </c>
+      <c r="O126" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="127" spans="4:15">
+      <c r="D127" t="s">
+        <v>33</v>
+      </c>
+      <c r="E127" t="s">
+        <v>43</v>
+      </c>
+      <c r="F127">
+        <v>33041260110504</v>
+      </c>
+      <c r="G127" t="s">
+        <v>79</v>
+      </c>
+      <c r="H127">
+        <v>20</v>
+      </c>
+      <c r="I127" t="s">
+        <v>105</v>
+      </c>
+      <c r="K127" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L127">
+        <v>33041260110504</v>
+      </c>
+      <c r="M127" t="s">
+        <v>161</v>
+      </c>
+      <c r="O127" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="128" spans="4:15">
+      <c r="D128" t="s">
+        <v>33</v>
+      </c>
+      <c r="E128" t="s">
+        <v>43</v>
+      </c>
+      <c r="F128">
+        <v>33041260091534</v>
+      </c>
+      <c r="G128" t="s">
+        <v>80</v>
+      </c>
+      <c r="H128">
+        <v>20</v>
+      </c>
+      <c r="I128" t="s">
+        <v>105</v>
+      </c>
+      <c r="K128" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L128">
+        <v>33041260091534</v>
+      </c>
+      <c r="M128" t="s">
+        <v>182</v>
+      </c>
+      <c r="O128" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="129" spans="4:15">
+      <c r="D129" t="s">
+        <v>33</v>
+      </c>
+      <c r="E129" t="s">
+        <v>43</v>
+      </c>
+      <c r="F129">
+        <v>33041260091372</v>
+      </c>
+      <c r="G129" t="s">
+        <v>81</v>
+      </c>
+      <c r="H129">
+        <v>20</v>
+      </c>
+      <c r="I129" t="s">
+        <v>105</v>
+      </c>
+      <c r="K129" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L129">
+        <v>33041260091372</v>
+      </c>
+      <c r="M129" t="s">
+        <v>183</v>
+      </c>
+      <c r="O129" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="130" spans="4:15">
+      <c r="D130" t="s">
+        <v>33</v>
+      </c>
+      <c r="E130" t="s">
+        <v>43</v>
+      </c>
+      <c r="F130">
+        <v>33041260091291</v>
+      </c>
+      <c r="G130" t="s">
+        <v>82</v>
+      </c>
+      <c r="H130">
+        <v>20</v>
+      </c>
+      <c r="I130" t="s">
+        <v>105</v>
+      </c>
+      <c r="K130" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L130">
+        <v>33041260091291</v>
+      </c>
+      <c r="M130" t="s">
+        <v>161</v>
+      </c>
+      <c r="O130" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="131" spans="4:15">
+      <c r="D131" t="s">
+        <v>33</v>
+      </c>
+      <c r="E131" t="s">
+        <v>43</v>
+      </c>
+      <c r="F131">
+        <v>33041260091453</v>
+      </c>
+      <c r="G131" t="s">
+        <v>83</v>
+      </c>
+      <c r="H131">
+        <v>20</v>
+      </c>
+      <c r="I131" t="s">
+        <v>105</v>
+      </c>
+      <c r="K131" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L131">
+        <v>33041260091453</v>
+      </c>
+      <c r="M131" t="s">
+        <v>161</v>
+      </c>
+      <c r="O131" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="132" spans="4:15">
+      <c r="D132" t="s">
+        <v>33</v>
+      </c>
+      <c r="E132" t="s">
+        <v>43</v>
+      </c>
+      <c r="F132">
+        <v>33041260110423</v>
+      </c>
+      <c r="G132" t="s">
         <v>84</v>
       </c>
-      <c r="K116" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="L116" t="s">
-        <v>134</v>
-      </c>
-      <c r="M116" t="s">
-        <v>141</v>
-      </c>
-      <c r="O116" t="s">
-        <v>156</v>
+      <c r="H132">
+        <v>20</v>
+      </c>
+      <c r="I132" t="s">
+        <v>105</v>
+      </c>
+      <c r="K132" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L132">
+        <v>33041260110423</v>
+      </c>
+      <c r="M132" t="s">
+        <v>161</v>
+      </c>
+      <c r="O132" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="133" spans="4:15">
+      <c r="D133" t="s">
+        <v>33</v>
+      </c>
+      <c r="E133" t="s">
+        <v>43</v>
+      </c>
+      <c r="F133">
+        <v>33041260091615</v>
+      </c>
+      <c r="G133" t="s">
+        <v>85</v>
+      </c>
+      <c r="H133">
+        <v>20</v>
+      </c>
+      <c r="I133" t="s">
+        <v>105</v>
+      </c>
+      <c r="K133" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L133">
+        <v>33041260091615</v>
+      </c>
+      <c r="M133" t="s">
+        <v>161</v>
+      </c>
+      <c r="O133" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="134" spans="4:15">
+      <c r="D134" t="s">
+        <v>33</v>
+      </c>
+      <c r="E134" t="s">
+        <v>43</v>
+      </c>
+      <c r="F134">
+        <v>33041260110695</v>
+      </c>
+      <c r="G134">
+        <v>6658103</v>
+      </c>
+      <c r="H134">
+        <v>20</v>
+      </c>
+      <c r="I134" t="s">
+        <v>105</v>
+      </c>
+      <c r="K134" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L134">
+        <v>33041260110695</v>
+      </c>
+      <c r="M134" t="s">
+        <v>184</v>
+      </c>
+      <c r="O134" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="135" spans="4:15">
+      <c r="D135" t="s">
+        <v>33</v>
+      </c>
+      <c r="E135" t="s">
+        <v>43</v>
+      </c>
+      <c r="F135">
+        <v>33041260026392</v>
+      </c>
+      <c r="G135">
+        <v>3610360</v>
+      </c>
+      <c r="H135">
+        <v>20</v>
+      </c>
+      <c r="I135" t="s">
+        <v>105</v>
+      </c>
+      <c r="K135" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L135">
+        <v>600990</v>
+      </c>
+      <c r="M135" t="s">
+        <v>185</v>
+      </c>
+      <c r="O135" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="136" spans="4:15">
+      <c r="D136" t="s">
+        <v>33</v>
+      </c>
+      <c r="E136" t="s">
+        <v>43</v>
+      </c>
+      <c r="F136">
+        <v>33041260180634</v>
+      </c>
+      <c r="G136" t="s">
+        <v>86</v>
+      </c>
+      <c r="H136">
+        <v>20</v>
+      </c>
+      <c r="I136" t="s">
+        <v>105</v>
+      </c>
+      <c r="K136" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L136">
+        <v>25856654889</v>
+      </c>
+      <c r="M136" t="s">
+        <v>186</v>
+      </c>
+      <c r="O136" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4842,6 +5587,26 @@
     <hyperlink ref="K114" r:id="rId112"/>
     <hyperlink ref="K115" r:id="rId113"/>
     <hyperlink ref="K116" r:id="rId114"/>
+    <hyperlink ref="K117" r:id="rId115"/>
+    <hyperlink ref="K118" r:id="rId116"/>
+    <hyperlink ref="K119" r:id="rId117"/>
+    <hyperlink ref="K120" r:id="rId118"/>
+    <hyperlink ref="K121" r:id="rId119"/>
+    <hyperlink ref="K122" r:id="rId120"/>
+    <hyperlink ref="K123" r:id="rId121"/>
+    <hyperlink ref="K124" r:id="rId122"/>
+    <hyperlink ref="K125" r:id="rId123"/>
+    <hyperlink ref="K126" r:id="rId124"/>
+    <hyperlink ref="K127" r:id="rId125"/>
+    <hyperlink ref="K128" r:id="rId126"/>
+    <hyperlink ref="K129" r:id="rId127"/>
+    <hyperlink ref="K130" r:id="rId128"/>
+    <hyperlink ref="K131" r:id="rId129"/>
+    <hyperlink ref="K132" r:id="rId130"/>
+    <hyperlink ref="K133" r:id="rId131"/>
+    <hyperlink ref="K134" r:id="rId132"/>
+    <hyperlink ref="K135" r:id="rId133"/>
+    <hyperlink ref="K136" r:id="rId134"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Refactor login functionality for municipalities
</commit_message>
<xml_diff>
--- a/ValidarAcessoPrefeituras.xlsx
+++ b/ValidarAcessoPrefeituras.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="204">
   <si>
     <t>Status</t>
   </si>
@@ -286,9 +286,6 @@
     <t xml:space="preserve">0825503-0 </t>
   </si>
   <si>
-    <t>731835904282</t>
-  </si>
-  <si>
     <t>130086-5</t>
   </si>
   <si>
@@ -512,21 +509,6 @@
   </si>
   <si>
     <t>093732</t>
-  </si>
-  <si>
-    <t>106240</t>
-  </si>
-  <si>
-    <t>208584</t>
-  </si>
-  <si>
-    <t>292044</t>
-  </si>
-  <si>
-    <t>349352</t>
-  </si>
-  <si>
-    <t>352093</t>
   </si>
   <si>
     <t>Via2024@</t>
@@ -1087,22 +1069,22 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="O2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1125,13 +1107,13 @@
         <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L3">
         <v>33041260113791</v>
@@ -1140,7 +1122,7 @@
         <v>33041260</v>
       </c>
       <c r="O3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1163,25 +1145,25 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L4">
         <v>33041260156768</v>
       </c>
       <c r="M4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="N4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="O4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1204,25 +1186,25 @@
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L5">
         <v>33041260134799</v>
       </c>
       <c r="M5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="N5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="O5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1245,22 +1227,22 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="O6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1283,22 +1265,22 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L7">
         <v>33041260129523</v>
       </c>
       <c r="M7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O7" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1321,22 +1303,22 @@
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N8" t="s">
+        <v>196</v>
+      </c>
+      <c r="O8" t="s">
         <v>202</v>
-      </c>
-      <c r="O8" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1359,22 +1341,22 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N9" t="s">
+        <v>196</v>
+      </c>
+      <c r="O9" t="s">
         <v>202</v>
-      </c>
-      <c r="O9" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1397,22 +1379,22 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N10" t="s">
+        <v>196</v>
+      </c>
+      <c r="O10" t="s">
         <v>202</v>
-      </c>
-      <c r="O10" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1435,22 +1417,22 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N11" t="s">
+        <v>196</v>
+      </c>
+      <c r="O11" t="s">
         <v>202</v>
-      </c>
-      <c r="O11" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1473,22 +1455,22 @@
         <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="O12" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1511,13 +1493,13 @@
         <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L13">
         <v>33041260151960</v>
@@ -1526,7 +1508,7 @@
         <v>783856</v>
       </c>
       <c r="O13" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1549,22 +1531,22 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M14" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="O14" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1587,25 +1569,25 @@
         <v>20</v>
       </c>
       <c r="I15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L15">
         <v>33041260109921</v>
       </c>
       <c r="M15" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="N15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="O15" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1628,22 +1610,22 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L16">
         <v>33041260193027</v>
       </c>
       <c r="M16" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="O16" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="3:15">
@@ -1666,22 +1648,22 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M17" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="O17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="3:15">
@@ -1704,25 +1686,25 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M18" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="N18" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="O18" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="3:15">
@@ -1745,25 +1727,25 @@
         <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L19">
         <v>25856654889</v>
       </c>
       <c r="M19" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="N19" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="O19" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="3:15">
@@ -1786,13 +1768,13 @@
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L20">
         <v>33041260127407</v>
@@ -1801,7 +1783,7 @@
         <v>1033</v>
       </c>
       <c r="O20" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="3:15">
@@ -1821,19 +1803,19 @@
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M21" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O21" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="3:15">
@@ -1853,19 +1835,19 @@
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M22" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O22" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="3:15">
@@ -1885,19 +1867,19 @@
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M23" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O23" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="3:15">
@@ -1917,19 +1899,19 @@
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M24" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O24" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="3:15">
@@ -1949,19 +1931,19 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M25" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O25" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="3:15">
@@ -1981,19 +1963,19 @@
         <v>3</v>
       </c>
       <c r="I26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M26" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O26" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="3:15">
@@ -2013,19 +1995,19 @@
         <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M27" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O27" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="3:15">
@@ -2045,19 +2027,19 @@
         <v>3</v>
       </c>
       <c r="I28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M28" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O28" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="3:15">
@@ -2077,19 +2059,19 @@
         <v>3</v>
       </c>
       <c r="I29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M29" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O29" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="3:15">
@@ -2109,19 +2091,19 @@
         <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M30" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O30" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="3:15">
@@ -2141,19 +2123,19 @@
         <v>3</v>
       </c>
       <c r="I31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M31" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O31" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="3:15">
@@ -2173,19 +2155,19 @@
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M32" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O32" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="4:15">
@@ -2205,19 +2187,19 @@
         <v>3</v>
       </c>
       <c r="I33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M33" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O33" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="4:15">
@@ -2237,19 +2219,19 @@
         <v>3</v>
       </c>
       <c r="I34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M34" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O34" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="4:15">
@@ -2269,19 +2251,19 @@
         <v>3</v>
       </c>
       <c r="I35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M35" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O35" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="4:15">
@@ -2301,19 +2283,19 @@
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M36" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O36" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="4:15">
@@ -2333,19 +2315,19 @@
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M37" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O37" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="4:15">
@@ -2365,19 +2347,19 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M38" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O38" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="4:15">
@@ -2397,19 +2379,19 @@
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M39" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O39" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="4:15">
@@ -2429,19 +2411,19 @@
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M40" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O40" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="4:15">
@@ -2461,19 +2443,19 @@
         <v>3</v>
       </c>
       <c r="I41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M41" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O41" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="4:15">
@@ -2493,19 +2475,19 @@
         <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M42" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O42" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="4:15">
@@ -2525,19 +2507,19 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M43" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O43" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="4:15">
@@ -2557,19 +2539,19 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M44" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O44" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45" spans="4:15">
@@ -2589,19 +2571,19 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M45" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O45" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="4:15">
@@ -2621,19 +2603,19 @@
         <v>3</v>
       </c>
       <c r="I46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M46" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O46" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="4:15">
@@ -2653,19 +2635,19 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M47" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O47" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="4:15">
@@ -2685,19 +2667,19 @@
         <v>3</v>
       </c>
       <c r="I48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M48" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O48" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="4:15">
@@ -2717,19 +2699,19 @@
         <v>3</v>
       </c>
       <c r="I49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M49" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O49" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="4:15">
@@ -2749,19 +2731,19 @@
         <v>3</v>
       </c>
       <c r="I50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M50" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O50" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="4:15">
@@ -2781,19 +2763,19 @@
         <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M51" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O51" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="4:15">
@@ -2813,19 +2795,19 @@
         <v>3</v>
       </c>
       <c r="I52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M52" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O52" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="4:15">
@@ -2845,19 +2827,19 @@
         <v>3</v>
       </c>
       <c r="I53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M53" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O53" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="4:15">
@@ -2877,19 +2859,19 @@
         <v>3</v>
       </c>
       <c r="I54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M54" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O54" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="4:15">
@@ -2909,19 +2891,19 @@
         <v>3</v>
       </c>
       <c r="I55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L55" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M55" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O55" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="4:15">
@@ -2941,19 +2923,19 @@
         <v>3</v>
       </c>
       <c r="I56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M56" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O56" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="4:15">
@@ -2973,19 +2955,19 @@
         <v>3</v>
       </c>
       <c r="I57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M57" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O57" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="4:15">
@@ -3005,19 +2987,19 @@
         <v>3</v>
       </c>
       <c r="I58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M58" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O58" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="4:15">
@@ -3037,19 +3019,19 @@
         <v>3</v>
       </c>
       <c r="I59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M59" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O59" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="4:15">
@@ -3069,19 +3051,19 @@
         <v>3</v>
       </c>
       <c r="I60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L60" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M60" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O60" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="4:15">
@@ -3101,19 +3083,19 @@
         <v>3</v>
       </c>
       <c r="I61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L61" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M61" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O61" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="4:15">
@@ -3133,19 +3115,19 @@
         <v>3</v>
       </c>
       <c r="I62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M62" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O62" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="4:15">
@@ -3165,19 +3147,19 @@
         <v>3</v>
       </c>
       <c r="I63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M63" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O63" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="64" spans="4:15">
@@ -3197,19 +3179,19 @@
         <v>3</v>
       </c>
       <c r="I64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L64" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M64" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O64" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="4:15">
@@ -3229,19 +3211,19 @@
         <v>3</v>
       </c>
       <c r="I65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M65" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O65" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="4:15">
@@ -3261,19 +3243,19 @@
         <v>3</v>
       </c>
       <c r="I66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L66" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M66" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O66" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="4:15">
@@ -3293,19 +3275,19 @@
         <v>3</v>
       </c>
       <c r="I67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M67" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O67" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="4:15">
@@ -3325,19 +3307,19 @@
         <v>3</v>
       </c>
       <c r="I68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L68" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M68" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O68" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="4:15">
@@ -3357,19 +3339,19 @@
         <v>3</v>
       </c>
       <c r="I69" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L69" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M69" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O69" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="4:15">
@@ -3389,19 +3371,19 @@
         <v>3</v>
       </c>
       <c r="I70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M70" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O70" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="4:15">
@@ -3421,19 +3403,19 @@
         <v>3</v>
       </c>
       <c r="I71" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L71" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M71" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O71" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="4:15">
@@ -3453,19 +3435,19 @@
         <v>3</v>
       </c>
       <c r="I72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L72" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M72" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O72" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="4:15">
@@ -3485,19 +3467,19 @@
         <v>3</v>
       </c>
       <c r="I73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L73" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M73" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O73" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="4:15">
@@ -3517,19 +3499,19 @@
         <v>3</v>
       </c>
       <c r="I74" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M74" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O74" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="4:15">
@@ -3549,19 +3531,19 @@
         <v>3</v>
       </c>
       <c r="I75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M75" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O75" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="4:15">
@@ -3581,19 +3563,19 @@
         <v>3</v>
       </c>
       <c r="I76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L76" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M76" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O76" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="4:15">
@@ -3613,19 +3595,19 @@
         <v>3</v>
       </c>
       <c r="I77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M77" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O77" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="78" spans="4:15">
@@ -3645,19 +3627,19 @@
         <v>3</v>
       </c>
       <c r="I78" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L78" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M78" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O78" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="4:15">
@@ -3677,19 +3659,19 @@
         <v>3</v>
       </c>
       <c r="I79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L79" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M79" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O79" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="4:15">
@@ -3709,19 +3691,19 @@
         <v>3</v>
       </c>
       <c r="I80" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M80" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O80" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="4:15">
@@ -3741,19 +3723,19 @@
         <v>3</v>
       </c>
       <c r="I81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L81" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M81" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O81" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="82" spans="4:15">
@@ -3773,19 +3755,19 @@
         <v>3</v>
       </c>
       <c r="I82" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M82" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O82" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="83" spans="4:15">
@@ -3805,19 +3787,19 @@
         <v>3</v>
       </c>
       <c r="I83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L83" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M83" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O83" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="4:15">
@@ -3837,19 +3819,19 @@
         <v>3</v>
       </c>
       <c r="I84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L84" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M84" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O84" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="85" spans="4:15">
@@ -3869,19 +3851,19 @@
         <v>3</v>
       </c>
       <c r="I85" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L85" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M85" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O85" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" spans="4:15">
@@ -3901,19 +3883,19 @@
         <v>3</v>
       </c>
       <c r="I86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L86" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M86" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O86" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="87" spans="4:15">
@@ -3933,19 +3915,19 @@
         <v>3</v>
       </c>
       <c r="I87" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M87" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O87" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88" spans="4:15">
@@ -3965,19 +3947,19 @@
         <v>3</v>
       </c>
       <c r="I88" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L88" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M88" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O88" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="89" spans="4:15">
@@ -3997,19 +3979,19 @@
         <v>3</v>
       </c>
       <c r="I89" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L89" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M89" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O89" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="4:15">
@@ -4029,19 +4011,19 @@
         <v>3</v>
       </c>
       <c r="I90" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L90" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M90" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O90" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="91" spans="4:15">
@@ -4061,19 +4043,19 @@
         <v>3</v>
       </c>
       <c r="I91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L91" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M91" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O91" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="4:15">
@@ -4093,19 +4075,19 @@
         <v>3</v>
       </c>
       <c r="I92" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L92" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M92" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O92" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="93" spans="4:15">
@@ -4125,19 +4107,19 @@
         <v>3</v>
       </c>
       <c r="I93" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L93" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M93" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O93" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" spans="4:15">
@@ -4157,19 +4139,19 @@
         <v>3</v>
       </c>
       <c r="I94" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L94" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M94" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O94" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="4:15">
@@ -4189,19 +4171,19 @@
         <v>3</v>
       </c>
       <c r="I95" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M95" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O95" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" spans="4:15">
@@ -4221,19 +4203,19 @@
         <v>3</v>
       </c>
       <c r="I96" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L96" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M96" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O96" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="4:15">
@@ -4253,19 +4235,19 @@
         <v>3</v>
       </c>
       <c r="I97" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L97" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M97" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O97" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="98" spans="4:15">
@@ -4285,19 +4267,19 @@
         <v>3</v>
       </c>
       <c r="I98" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L98" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M98" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O98" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="99" spans="4:15">
@@ -4317,19 +4299,19 @@
         <v>3</v>
       </c>
       <c r="I99" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M99" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O99" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="100" spans="4:15">
@@ -4349,19 +4331,19 @@
         <v>3</v>
       </c>
       <c r="I100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L100" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M100" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O100" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="4:15">
@@ -4381,19 +4363,19 @@
         <v>3</v>
       </c>
       <c r="I101" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L101" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M101" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="O101" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="4:15">
@@ -4413,19 +4395,19 @@
         <v>12</v>
       </c>
       <c r="I102" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L102">
         <v>104321</v>
       </c>
       <c r="M102" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O102" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="4:15">
@@ -4445,19 +4427,19 @@
         <v>12</v>
       </c>
       <c r="I103" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L103" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M103" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O103" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="4:15">
@@ -4477,19 +4459,19 @@
         <v>12</v>
       </c>
       <c r="I104" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L104" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M104" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O104" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="4:15">
@@ -4509,19 +4491,19 @@
         <v>12</v>
       </c>
       <c r="I105" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L105" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M105" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O105" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" spans="4:15">
@@ -4541,19 +4523,19 @@
         <v>12</v>
       </c>
       <c r="I106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L106" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M106" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O106" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="4:15">
@@ -4573,19 +4555,19 @@
         <v>12</v>
       </c>
       <c r="I107" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L107" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M107" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O107" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="108" spans="4:15">
@@ -4605,19 +4587,19 @@
         <v>12</v>
       </c>
       <c r="I108" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K108" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L108">
         <v>106351</v>
       </c>
       <c r="M108" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O108" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="109" spans="4:15">
@@ -4637,19 +4619,19 @@
         <v>12</v>
       </c>
       <c r="I109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L109">
         <v>126415</v>
       </c>
       <c r="M109" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O109" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" spans="4:15">
@@ -4669,19 +4651,19 @@
         <v>12</v>
       </c>
       <c r="I110" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K110" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L110">
         <v>134398</v>
       </c>
       <c r="M110" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O110" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="4:15">
@@ -4701,19 +4683,19 @@
         <v>12</v>
       </c>
       <c r="I111" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L111" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M111" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="O111" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="112" spans="4:15">
@@ -4733,19 +4715,19 @@
         <v>12</v>
       </c>
       <c r="I112" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L112" t="s">
-        <v>166</v>
+        <v>147</v>
+      </c>
+      <c r="L112">
+        <v>106240</v>
       </c>
       <c r="M112" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="O112" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="113" spans="4:15">
@@ -4765,19 +4747,19 @@
         <v>12</v>
       </c>
       <c r="I113" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K113" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L113" t="s">
-        <v>167</v>
+        <v>147</v>
+      </c>
+      <c r="L113">
+        <v>208584</v>
       </c>
       <c r="M113" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="O113" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="4:15">
@@ -4797,19 +4779,19 @@
         <v>12</v>
       </c>
       <c r="I114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K114" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L114" t="s">
-        <v>168</v>
+        <v>147</v>
+      </c>
+      <c r="L114">
+        <v>292044</v>
       </c>
       <c r="M114" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="O114" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="4:15">
@@ -4829,19 +4811,19 @@
         <v>12</v>
       </c>
       <c r="I115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L115" t="s">
-        <v>169</v>
+        <v>147</v>
+      </c>
+      <c r="L115">
+        <v>349352</v>
       </c>
       <c r="M115" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="O115" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="4:15">
@@ -4861,19 +4843,19 @@
         <v>12</v>
       </c>
       <c r="I116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="L116" t="s">
-        <v>170</v>
+        <v>147</v>
+      </c>
+      <c r="L116">
+        <v>352093</v>
       </c>
       <c r="M116" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="O116" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="4:15">
@@ -4893,19 +4875,19 @@
         <v>20</v>
       </c>
       <c r="I117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L117">
         <v>500200</v>
       </c>
       <c r="M117" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="O117" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="4:15">
@@ -4925,19 +4907,19 @@
         <v>20</v>
       </c>
       <c r="I118" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L118">
         <v>150230</v>
       </c>
       <c r="M118" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="O118" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="4:15">
@@ -4957,19 +4939,19 @@
         <v>20</v>
       </c>
       <c r="I119" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K119" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L119">
         <v>740220</v>
       </c>
       <c r="M119" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="O119" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="120" spans="4:15">
@@ -4989,19 +4971,19 @@
         <v>20</v>
       </c>
       <c r="I120" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K120" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L120">
         <v>123392</v>
       </c>
       <c r="M120" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="O120" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="121" spans="4:15">
@@ -5021,19 +5003,19 @@
         <v>20</v>
       </c>
       <c r="I121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L121">
         <v>193237</v>
       </c>
       <c r="M121" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O121" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="4:15">
@@ -5053,19 +5035,19 @@
         <v>20</v>
       </c>
       <c r="I122" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L122">
         <v>172181</v>
       </c>
       <c r="M122" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="O122" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="123" spans="4:15">
@@ -5085,19 +5067,19 @@
         <v>20</v>
       </c>
       <c r="I123" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K123" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L123">
         <v>149207</v>
       </c>
       <c r="M123" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O123" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="124" spans="4:15">
@@ -5117,19 +5099,19 @@
         <v>20</v>
       </c>
       <c r="I124" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L124">
         <v>402622</v>
       </c>
       <c r="M124" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="O124" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="125" spans="4:15">
@@ -5149,19 +5131,19 @@
         <v>20</v>
       </c>
       <c r="I125" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L125">
         <v>33041260091020</v>
       </c>
       <c r="M125" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="O125" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="4:15">
@@ -5181,19 +5163,19 @@
         <v>20</v>
       </c>
       <c r="I126" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K126" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L126">
         <v>33041260091100</v>
       </c>
       <c r="M126" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="O126" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="4:15">
@@ -5213,19 +5195,19 @@
         <v>20</v>
       </c>
       <c r="I127" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L127">
         <v>33041260110504</v>
       </c>
       <c r="M127" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O127" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="128" spans="4:15">
@@ -5245,19 +5227,19 @@
         <v>20</v>
       </c>
       <c r="I128" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K128" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L128">
         <v>33041260091534</v>
       </c>
       <c r="M128" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="O128" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="129" spans="4:15">
@@ -5277,19 +5259,19 @@
         <v>20</v>
       </c>
       <c r="I129" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K129" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L129">
         <v>33041260091372</v>
       </c>
       <c r="M129" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="O129" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="130" spans="4:15">
@@ -5309,19 +5291,19 @@
         <v>20</v>
       </c>
       <c r="I130" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K130" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L130">
         <v>33041260091291</v>
       </c>
       <c r="M130" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O130" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="131" spans="4:15">
@@ -5341,19 +5323,19 @@
         <v>20</v>
       </c>
       <c r="I131" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K131" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L131">
         <v>33041260091453</v>
       </c>
       <c r="M131" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O131" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="132" spans="4:15">
@@ -5373,19 +5355,19 @@
         <v>20</v>
       </c>
       <c r="I132" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K132" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L132">
         <v>33041260110423</v>
       </c>
       <c r="M132" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O132" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="4:15">
@@ -5405,19 +5387,19 @@
         <v>20</v>
       </c>
       <c r="I133" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K133" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L133">
         <v>33041260091615</v>
       </c>
       <c r="M133" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="O133" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="4:15">
@@ -5437,19 +5419,19 @@
         <v>20</v>
       </c>
       <c r="I134" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K134" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L134">
         <v>33041260110695</v>
       </c>
       <c r="M134" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="O134" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" spans="4:15">
@@ -5469,19 +5451,19 @@
         <v>20</v>
       </c>
       <c r="I135" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L135">
         <v>600990</v>
       </c>
       <c r="M135" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="O135" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="136" spans="4:15">
@@ -5501,19 +5483,19 @@
         <v>20</v>
       </c>
       <c r="I136" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K136" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L136">
         <v>25856654889</v>
       </c>
       <c r="M136" t="s">
+        <v>194</v>
+      </c>
+      <c r="O136" t="s">
         <v>200</v>
-      </c>
-      <c r="O136" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="137" spans="4:15">
@@ -5533,13 +5515,16 @@
         <v>20</v>
       </c>
       <c r="I137" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K137" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L137">
         <v>731835900880</v>
+      </c>
+      <c r="O137" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="138" spans="4:15">
@@ -5559,13 +5544,16 @@
         <v>20</v>
       </c>
       <c r="I138" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K138" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L138">
         <v>731835900708</v>
+      </c>
+      <c r="O138" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="139" spans="4:15">
@@ -5585,13 +5573,16 @@
         <v>20</v>
       </c>
       <c r="I139" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K139" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L139">
         <v>731835901003</v>
+      </c>
+      <c r="O139" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="140" spans="4:15">
@@ -5611,13 +5602,16 @@
         <v>20</v>
       </c>
       <c r="I140" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K140" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L140">
         <v>731835900538</v>
+      </c>
+      <c r="O140" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="141" spans="4:15">
@@ -5637,13 +5631,16 @@
         <v>20</v>
       </c>
       <c r="I141" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K141" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L141">
         <v>731835901429</v>
+      </c>
+      <c r="O141" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="142" spans="4:15">
@@ -5663,13 +5660,16 @@
         <v>20</v>
       </c>
       <c r="I142" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K142" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L142">
         <v>731835901771</v>
+      </c>
+      <c r="O142" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="4:15">
@@ -5689,13 +5689,16 @@
         <v>20</v>
       </c>
       <c r="I143" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K143" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L143">
         <v>731835901933</v>
+      </c>
+      <c r="O143" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="4:15">
@@ -5715,16 +5718,19 @@
         <v>20</v>
       </c>
       <c r="I144" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K144" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L144">
         <v>731835902743</v>
       </c>
-    </row>
-    <row r="145" spans="4:12">
+      <c r="O144" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="145" spans="4:15">
       <c r="D145" t="s">
         <v>34</v>
       </c>
@@ -5741,16 +5747,19 @@
         <v>20</v>
       </c>
       <c r="I145" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K145" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L145">
         <v>731835903391</v>
       </c>
-    </row>
-    <row r="146" spans="4:12">
+      <c r="O145" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="146" spans="4:15">
       <c r="D146" t="s">
         <v>34</v>
       </c>
@@ -5767,16 +5776,19 @@
         <v>20</v>
       </c>
       <c r="I146" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K146" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L146">
         <v>731835902824</v>
       </c>
-    </row>
-    <row r="147" spans="4:12">
+      <c r="O146" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="147" spans="4:15">
       <c r="D147" t="s">
         <v>34</v>
       </c>
@@ -5793,16 +5805,19 @@
         <v>20</v>
       </c>
       <c r="I147" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K147" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L147">
         <v>731835902310</v>
       </c>
-    </row>
-    <row r="148" spans="4:12">
+      <c r="O147" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="148" spans="4:15">
       <c r="D148" t="s">
         <v>34</v>
       </c>
@@ -5819,16 +5834,19 @@
         <v>20</v>
       </c>
       <c r="I148" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K148" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L148">
         <v>731835903472</v>
       </c>
-    </row>
-    <row r="149" spans="4:12">
+      <c r="O148" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="149" spans="4:15">
       <c r="D149" t="s">
         <v>34</v>
       </c>
@@ -5845,16 +5863,19 @@
         <v>20</v>
       </c>
       <c r="I149" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K149" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L149">
         <v>731835902905</v>
       </c>
-    </row>
-    <row r="150" spans="4:12">
+      <c r="O149" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="150" spans="4:15">
       <c r="D150" t="s">
         <v>34</v>
       </c>
@@ -5871,16 +5892,19 @@
         <v>20</v>
       </c>
       <c r="I150" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K150" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L150">
         <v>731835903200</v>
       </c>
-    </row>
-    <row r="151" spans="4:12">
+      <c r="O150" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="151" spans="4:15">
       <c r="D151" t="s">
         <v>34</v>
       </c>
@@ -5897,16 +5921,19 @@
         <v>20</v>
       </c>
       <c r="I151" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K151" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L151">
         <v>731835903049</v>
       </c>
-    </row>
-    <row r="152" spans="4:12">
+      <c r="O151" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="152" spans="4:15">
       <c r="D152" t="s">
         <v>34</v>
       </c>
@@ -5923,16 +5950,19 @@
         <v>20</v>
       </c>
       <c r="I152" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K152" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L152">
         <v>731835902409</v>
       </c>
-    </row>
-    <row r="153" spans="4:12">
+      <c r="O152" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="153" spans="4:15">
       <c r="D153" t="s">
         <v>34</v>
       </c>
@@ -5949,16 +5979,19 @@
         <v>20</v>
       </c>
       <c r="I153" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K153" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L153">
         <v>731835903120</v>
       </c>
-    </row>
-    <row r="154" spans="4:12">
+      <c r="O153" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="154" spans="4:15">
       <c r="D154" t="s">
         <v>34</v>
       </c>
@@ -5975,16 +6008,19 @@
         <v>20</v>
       </c>
       <c r="I154" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K154" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L154">
         <v>731835903634</v>
       </c>
-    </row>
-    <row r="155" spans="4:12">
+      <c r="O154" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="155" spans="4:15">
       <c r="D155" t="s">
         <v>34</v>
       </c>
@@ -6001,16 +6037,19 @@
         <v>20</v>
       </c>
       <c r="I155" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K155" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L155">
         <v>731835902581</v>
       </c>
-    </row>
-    <row r="156" spans="4:12">
+      <c r="O155" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="156" spans="4:15">
       <c r="D156" t="s">
         <v>34</v>
       </c>
@@ -6027,16 +6066,19 @@
         <v>20</v>
       </c>
       <c r="I156" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K156" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L156">
         <v>731835903715</v>
       </c>
-    </row>
-    <row r="157" spans="4:12">
+      <c r="O156" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="157" spans="4:15">
       <c r="D157" t="s">
         <v>34</v>
       </c>
@@ -6053,16 +6095,19 @@
         <v>20</v>
       </c>
       <c r="I157" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K157" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L157">
         <v>731835903804</v>
       </c>
-    </row>
-    <row r="158" spans="4:12">
+      <c r="O157" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="158" spans="4:15">
       <c r="D158" t="s">
         <v>34</v>
       </c>
@@ -6079,16 +6124,19 @@
         <v>20</v>
       </c>
       <c r="I158" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K158" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L158">
         <v>731835902662</v>
       </c>
-    </row>
-    <row r="159" spans="4:12">
+      <c r="O158" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="159" spans="4:15">
       <c r="D159" t="s">
         <v>34</v>
       </c>
@@ -6105,16 +6153,19 @@
         <v>20</v>
       </c>
       <c r="I159" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K159" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L159">
         <v>731835900104</v>
       </c>
-    </row>
-    <row r="160" spans="4:12">
+      <c r="O159" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="160" spans="4:15">
       <c r="D160" t="s">
         <v>34</v>
       </c>
@@ -6124,23 +6175,26 @@
       <c r="F160">
         <v>33041260186918</v>
       </c>
-      <c r="G160" t="s">
-        <v>90</v>
+      <c r="G160">
+        <v>731835904282</v>
       </c>
       <c r="H160">
         <v>20</v>
       </c>
       <c r="I160" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K160" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="L160" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="161" spans="4:13">
+        <v>149</v>
+      </c>
+      <c r="L160">
+        <v>731835904282</v>
+      </c>
+      <c r="O160" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="161" spans="4:15">
       <c r="D161" t="s">
         <v>35</v>
       </c>
@@ -6151,25 +6205,28 @@
         <v>33041260162652</v>
       </c>
       <c r="G161" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H161">
         <v>25</v>
       </c>
       <c r="I161" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K161" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L161">
         <v>22153982804</v>
       </c>
       <c r="M161" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="162" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O161" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="162" spans="4:15">
       <c r="D162" t="s">
         <v>35</v>
       </c>
@@ -6186,19 +6243,22 @@
         <v>25</v>
       </c>
       <c r="I162" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K162" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L162">
         <v>22153982804</v>
       </c>
       <c r="M162" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="163" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O162" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="163" spans="4:15">
       <c r="D163" t="s">
         <v>35</v>
       </c>
@@ -6215,19 +6275,22 @@
         <v>25</v>
       </c>
       <c r="I163" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K163" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L163">
         <v>22153982804</v>
       </c>
       <c r="M163" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="164" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O163" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="164" spans="4:15">
       <c r="D164" t="s">
         <v>35</v>
       </c>
@@ -6244,19 +6307,22 @@
         <v>25</v>
       </c>
       <c r="I164" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K164" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L164">
         <v>22153982804</v>
       </c>
       <c r="M164" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="165" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O164" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="165" spans="4:15">
       <c r="D165" t="s">
         <v>35</v>
       </c>
@@ -6273,19 +6339,22 @@
         <v>25</v>
       </c>
       <c r="I165" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K165" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L165">
         <v>22153982804</v>
       </c>
       <c r="M165" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="166" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O165" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="166" spans="4:15">
       <c r="D166" t="s">
         <v>35</v>
       </c>
@@ -6302,19 +6371,22 @@
         <v>25</v>
       </c>
       <c r="I166" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K166" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L166">
         <v>22153982804</v>
       </c>
       <c r="M166" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="167" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O166" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="167" spans="4:15">
       <c r="D167" t="s">
         <v>35</v>
       </c>
@@ -6331,19 +6403,22 @@
         <v>25</v>
       </c>
       <c r="I167" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K167" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L167">
         <v>22153982804</v>
       </c>
       <c r="M167" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="168" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O167" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="168" spans="4:15">
       <c r="D168" t="s">
         <v>35</v>
       </c>
@@ -6360,19 +6435,22 @@
         <v>25</v>
       </c>
       <c r="I168" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K168" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L168">
         <v>22153982804</v>
       </c>
       <c r="M168" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="169" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O168" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="169" spans="4:15">
       <c r="D169" t="s">
         <v>35</v>
       </c>
@@ -6389,19 +6467,22 @@
         <v>25</v>
       </c>
       <c r="I169" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K169" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L169">
         <v>22153982804</v>
       </c>
       <c r="M169" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="170" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O169" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="170" spans="4:15">
       <c r="D170" t="s">
         <v>35</v>
       </c>
@@ -6418,19 +6499,22 @@
         <v>25</v>
       </c>
       <c r="I170" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L170">
         <v>22153982804</v>
       </c>
       <c r="M170" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="171" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O170" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="171" spans="4:15">
       <c r="D171" t="s">
         <v>35</v>
       </c>
@@ -6447,19 +6531,22 @@
         <v>25</v>
       </c>
       <c r="I171" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K171" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L171">
         <v>22153982804</v>
       </c>
       <c r="M171" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="172" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O171" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="172" spans="4:15">
       <c r="D172" t="s">
         <v>35</v>
       </c>
@@ -6470,25 +6557,28 @@
         <v>33041260175800</v>
       </c>
       <c r="G172" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H172">
         <v>25</v>
       </c>
       <c r="I172" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K172" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L172">
         <v>22153982804</v>
       </c>
       <c r="M172" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="173" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O172" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="173" spans="4:15">
       <c r="D173" t="s">
         <v>35</v>
       </c>
@@ -6499,25 +6589,28 @@
         <v>33041260175207</v>
       </c>
       <c r="G173" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H173">
         <v>25</v>
       </c>
       <c r="I173" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K173" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L173">
         <v>22153982804</v>
       </c>
       <c r="M173" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="174" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O173" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="174" spans="4:15">
       <c r="D174" t="s">
         <v>35</v>
       </c>
@@ -6528,25 +6621,28 @@
         <v>33041260178060</v>
       </c>
       <c r="G174" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H174">
         <v>25</v>
       </c>
       <c r="I174" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K174" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L174">
         <v>22153982804</v>
       </c>
       <c r="M174" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="175" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O174" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="175" spans="4:15">
       <c r="D175" t="s">
         <v>35</v>
       </c>
@@ -6557,25 +6653,28 @@
         <v>33041260181363</v>
       </c>
       <c r="G175" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H175">
         <v>25</v>
       </c>
       <c r="I175" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K175" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L175">
         <v>22153982804</v>
       </c>
       <c r="M175" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="176" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O175" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="176" spans="4:15">
       <c r="D176" t="s">
         <v>35</v>
       </c>
@@ -6586,25 +6685,28 @@
         <v>33041260161508</v>
       </c>
       <c r="G176" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H176">
         <v>25</v>
       </c>
       <c r="I176" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K176" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L176">
         <v>22153982804</v>
       </c>
       <c r="M176" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="177" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O176" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="177" spans="4:15">
       <c r="D177" t="s">
         <v>35</v>
       </c>
@@ -6615,25 +6717,28 @@
         <v>33041260075091</v>
       </c>
       <c r="G177" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H177">
         <v>25</v>
       </c>
       <c r="I177" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K177" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L177">
         <v>22153982804</v>
       </c>
       <c r="M177" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="178" spans="4:13">
+        <v>195</v>
+      </c>
+      <c r="O177" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="178" spans="4:15">
       <c r="D178" t="s">
         <v>35</v>
       </c>
@@ -6650,16 +6755,19 @@
         <v>25</v>
       </c>
       <c r="I178" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K178" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L178">
         <v>22153982804</v>
       </c>
       <c r="M178" t="s">
-        <v>201</v>
+        <v>195</v>
+      </c>
+      <c r="O178" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Enable headless mode and adjust log level for ChromeOptions
</commit_message>
<xml_diff>
--- a/ValidarAcessoPrefeituras.xlsx
+++ b/ValidarAcessoPrefeituras.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="206">
   <si>
     <t>Status</t>
   </si>
@@ -610,22 +610,28 @@
     <t>NÃO</t>
   </si>
   <si>
-    <t>LOGIN INVÁLIDO</t>
+    <t>VÁLIDO</t>
+  </si>
+  <si>
+    <t>PÁGINA NÃO ABRIU</t>
+  </si>
+  <si>
+    <t>VERIFICAR FORMA DE ACESSO</t>
+  </si>
+  <si>
+    <t>LOGIN INVALIDO</t>
+  </si>
+  <si>
+    <t>ACESSO POR CERTIFICADO</t>
+  </si>
+  <si>
+    <t>FALTA INFORMAÇÃO</t>
   </si>
   <si>
     <t>LOGIN VÁLIDO</t>
   </si>
   <si>
-    <t>VERIFICAR FORMA DE ACESSO</t>
-  </si>
-  <si>
-    <t>ACESSO POR CERTIFICADO</t>
-  </si>
-  <si>
     <t>Pulando</t>
-  </si>
-  <si>
-    <t>VÁLIDO</t>
   </si>
 </sst>
 </file>
@@ -1083,6 +1089,9 @@
       <c r="M2" t="s">
         <v>165</v>
       </c>
+      <c r="O2" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="3" spans="1:15">
       <c r="C3">
@@ -1118,6 +1127,9 @@
       <c r="M3">
         <v>33041260</v>
       </c>
+      <c r="O3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="C4">
@@ -1156,6 +1168,9 @@
       <c r="N4" t="s">
         <v>196</v>
       </c>
+      <c r="O4" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="5" spans="1:15">
       <c r="C5">
@@ -1194,6 +1209,9 @@
       <c r="N5" t="s">
         <v>197</v>
       </c>
+      <c r="O5" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="C6">
@@ -1229,6 +1247,9 @@
       <c r="M6" t="s">
         <v>168</v>
       </c>
+      <c r="O6" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
       <c r="C7">
@@ -1264,6 +1285,9 @@
       <c r="M7" t="s">
         <v>169</v>
       </c>
+      <c r="O7" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="C8">
@@ -1299,6 +1323,9 @@
       <c r="N8" t="s">
         <v>196</v>
       </c>
+      <c r="O8" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="9" spans="1:15">
       <c r="C9">
@@ -1334,6 +1361,9 @@
       <c r="N9" t="s">
         <v>196</v>
       </c>
+      <c r="O9" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="C10">
@@ -1369,6 +1399,9 @@
       <c r="N10" t="s">
         <v>196</v>
       </c>
+      <c r="O10" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="C11">
@@ -1404,6 +1437,9 @@
       <c r="N11" t="s">
         <v>196</v>
       </c>
+      <c r="O11" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="C12">
@@ -1439,6 +1475,9 @@
       <c r="M12" t="s">
         <v>170</v>
       </c>
+      <c r="O12" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="C13">
@@ -1474,6 +1513,9 @@
       <c r="M13">
         <v>783856</v>
       </c>
+      <c r="O13" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="14" spans="1:15">
       <c r="C14">
@@ -1509,6 +1551,9 @@
       <c r="M14" t="s">
         <v>171</v>
       </c>
+      <c r="O14" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="C15">
@@ -1547,6 +1592,9 @@
       <c r="N15" t="s">
         <v>196</v>
       </c>
+      <c r="O15" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="C16">
@@ -1582,6 +1630,9 @@
       <c r="M16" t="s">
         <v>173</v>
       </c>
+      <c r="O16" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="17" spans="3:15">
       <c r="C17">
@@ -1617,6 +1668,9 @@
       <c r="M17" t="s">
         <v>165</v>
       </c>
+      <c r="O17" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="18" spans="3:15">
       <c r="C18">
@@ -1655,6 +1709,9 @@
       <c r="N18" t="s">
         <v>196</v>
       </c>
+      <c r="O18" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="19" spans="3:15">
       <c r="C19">
@@ -1693,6 +1750,9 @@
       <c r="N19" t="s">
         <v>196</v>
       </c>
+      <c r="O19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="20" spans="3:15">
       <c r="C20">
@@ -1728,6 +1788,9 @@
       <c r="M20">
         <v>1033</v>
       </c>
+      <c r="O20" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="21" spans="3:15">
       <c r="D21" t="s">
@@ -1758,7 +1821,7 @@
         <v>175</v>
       </c>
       <c r="O21" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="3:15">
@@ -1790,7 +1853,7 @@
         <v>175</v>
       </c>
       <c r="O22" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="3:15">
@@ -1822,7 +1885,7 @@
         <v>175</v>
       </c>
       <c r="O23" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="3:15">
@@ -1854,7 +1917,7 @@
         <v>175</v>
       </c>
       <c r="O24" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="3:15">
@@ -1886,7 +1949,7 @@
         <v>175</v>
       </c>
       <c r="O25" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="3:15">
@@ -1918,7 +1981,7 @@
         <v>175</v>
       </c>
       <c r="O26" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="3:15">
@@ -1950,7 +2013,7 @@
         <v>175</v>
       </c>
       <c r="O27" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="3:15">
@@ -1982,7 +2045,7 @@
         <v>175</v>
       </c>
       <c r="O28" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="3:15">
@@ -2014,7 +2077,7 @@
         <v>175</v>
       </c>
       <c r="O29" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="3:15">
@@ -2046,7 +2109,7 @@
         <v>175</v>
       </c>
       <c r="O30" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="3:15">
@@ -2078,7 +2141,7 @@
         <v>175</v>
       </c>
       <c r="O31" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="3:15">
@@ -2110,7 +2173,7 @@
         <v>175</v>
       </c>
       <c r="O32" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="4:15">
@@ -2142,7 +2205,7 @@
         <v>175</v>
       </c>
       <c r="O33" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="4:15">
@@ -2174,7 +2237,7 @@
         <v>175</v>
       </c>
       <c r="O34" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="4:15">
@@ -2206,7 +2269,7 @@
         <v>175</v>
       </c>
       <c r="O35" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="4:15">
@@ -2238,7 +2301,7 @@
         <v>175</v>
       </c>
       <c r="O36" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="4:15">
@@ -2270,7 +2333,7 @@
         <v>175</v>
       </c>
       <c r="O37" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="4:15">
@@ -2302,7 +2365,7 @@
         <v>175</v>
       </c>
       <c r="O38" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="4:15">
@@ -2334,7 +2397,7 @@
         <v>175</v>
       </c>
       <c r="O39" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="4:15">
@@ -2366,7 +2429,7 @@
         <v>175</v>
       </c>
       <c r="O40" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="41" spans="4:15">
@@ -2398,7 +2461,7 @@
         <v>175</v>
       </c>
       <c r="O41" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="4:15">
@@ -2430,7 +2493,7 @@
         <v>175</v>
       </c>
       <c r="O42" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="4:15">
@@ -2462,7 +2525,7 @@
         <v>175</v>
       </c>
       <c r="O43" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="4:15">
@@ -2494,7 +2557,7 @@
         <v>175</v>
       </c>
       <c r="O44" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="4:15">
@@ -2526,7 +2589,7 @@
         <v>175</v>
       </c>
       <c r="O45" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="4:15">
@@ -2558,7 +2621,7 @@
         <v>175</v>
       </c>
       <c r="O46" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="4:15">
@@ -2590,7 +2653,7 @@
         <v>175</v>
       </c>
       <c r="O47" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="4:15">
@@ -2622,7 +2685,7 @@
         <v>175</v>
       </c>
       <c r="O48" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="4:15">
@@ -2654,7 +2717,7 @@
         <v>175</v>
       </c>
       <c r="O49" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="4:15">
@@ -2686,7 +2749,7 @@
         <v>175</v>
       </c>
       <c r="O50" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="51" spans="4:15">
@@ -2718,7 +2781,7 @@
         <v>175</v>
       </c>
       <c r="O51" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="4:15">
@@ -2750,7 +2813,7 @@
         <v>175</v>
       </c>
       <c r="O52" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="4:15">
@@ -2782,7 +2845,7 @@
         <v>175</v>
       </c>
       <c r="O53" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="4:15">
@@ -2814,7 +2877,7 @@
         <v>175</v>
       </c>
       <c r="O54" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="4:15">
@@ -2846,7 +2909,7 @@
         <v>175</v>
       </c>
       <c r="O55" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="4:15">
@@ -2878,7 +2941,7 @@
         <v>175</v>
       </c>
       <c r="O56" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="4:15">
@@ -2910,7 +2973,7 @@
         <v>175</v>
       </c>
       <c r="O57" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" spans="4:15">
@@ -2942,7 +3005,7 @@
         <v>175</v>
       </c>
       <c r="O58" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" spans="4:15">
@@ -2974,7 +3037,7 @@
         <v>175</v>
       </c>
       <c r="O59" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="4:15">
@@ -3006,7 +3069,7 @@
         <v>175</v>
       </c>
       <c r="O60" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="61" spans="4:15">
@@ -3038,7 +3101,7 @@
         <v>175</v>
       </c>
       <c r="O61" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="4:15">
@@ -3070,7 +3133,7 @@
         <v>175</v>
       </c>
       <c r="O62" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="4:15">
@@ -3102,7 +3165,7 @@
         <v>175</v>
       </c>
       <c r="O63" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="4:15">
@@ -3134,7 +3197,7 @@
         <v>175</v>
       </c>
       <c r="O64" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="4:15">
@@ -3166,7 +3229,7 @@
         <v>175</v>
       </c>
       <c r="O65" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="4:15">
@@ -3198,7 +3261,7 @@
         <v>175</v>
       </c>
       <c r="O66" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="4:15">
@@ -3230,7 +3293,7 @@
         <v>175</v>
       </c>
       <c r="O67" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="4:15">
@@ -3262,7 +3325,7 @@
         <v>175</v>
       </c>
       <c r="O68" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="4:15">
@@ -3294,7 +3357,7 @@
         <v>175</v>
       </c>
       <c r="O69" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="4:15">
@@ -3326,7 +3389,7 @@
         <v>175</v>
       </c>
       <c r="O70" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="4:15">
@@ -3358,7 +3421,7 @@
         <v>175</v>
       </c>
       <c r="O71" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="4:15">
@@ -3390,7 +3453,7 @@
         <v>175</v>
       </c>
       <c r="O72" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="4:15">
@@ -3422,7 +3485,7 @@
         <v>175</v>
       </c>
       <c r="O73" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="4:15">
@@ -3454,7 +3517,7 @@
         <v>175</v>
       </c>
       <c r="O74" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="4:15">
@@ -3486,7 +3549,7 @@
         <v>175</v>
       </c>
       <c r="O75" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="4:15">
@@ -3518,7 +3581,7 @@
         <v>175</v>
       </c>
       <c r="O76" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="4:15">
@@ -3550,7 +3613,7 @@
         <v>175</v>
       </c>
       <c r="O77" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="4:15">
@@ -3582,7 +3645,7 @@
         <v>175</v>
       </c>
       <c r="O78" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="79" spans="4:15">
@@ -3614,7 +3677,7 @@
         <v>175</v>
       </c>
       <c r="O79" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" spans="4:15">
@@ -3646,7 +3709,7 @@
         <v>175</v>
       </c>
       <c r="O80" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="81" spans="4:15">
@@ -3678,7 +3741,7 @@
         <v>175</v>
       </c>
       <c r="O81" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="4:15">
@@ -3710,7 +3773,7 @@
         <v>175</v>
       </c>
       <c r="O82" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="4:15">
@@ -3742,7 +3805,7 @@
         <v>175</v>
       </c>
       <c r="O83" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="84" spans="4:15">
@@ -3774,7 +3837,7 @@
         <v>175</v>
       </c>
       <c r="O84" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="4:15">
@@ -3806,7 +3869,7 @@
         <v>175</v>
       </c>
       <c r="O85" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="4:15">
@@ -3838,7 +3901,7 @@
         <v>175</v>
       </c>
       <c r="O86" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="4:15">
@@ -3870,7 +3933,7 @@
         <v>175</v>
       </c>
       <c r="O87" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="88" spans="4:15">
@@ -3902,7 +3965,7 @@
         <v>175</v>
       </c>
       <c r="O88" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="4:15">
@@ -3934,7 +3997,7 @@
         <v>175</v>
       </c>
       <c r="O89" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="4:15">
@@ -3966,7 +4029,7 @@
         <v>175</v>
       </c>
       <c r="O90" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="4:15">
@@ -3998,7 +4061,7 @@
         <v>175</v>
       </c>
       <c r="O91" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" spans="4:15">
@@ -4030,7 +4093,7 @@
         <v>175</v>
       </c>
       <c r="O92" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="4:15">
@@ -4062,7 +4125,7 @@
         <v>175</v>
       </c>
       <c r="O93" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="94" spans="4:15">
@@ -4094,7 +4157,7 @@
         <v>175</v>
       </c>
       <c r="O94" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="95" spans="4:15">
@@ -4126,7 +4189,7 @@
         <v>175</v>
       </c>
       <c r="O95" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="4:15">
@@ -4158,7 +4221,7 @@
         <v>175</v>
       </c>
       <c r="O96" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="4:15">
@@ -4190,7 +4253,7 @@
         <v>175</v>
       </c>
       <c r="O97" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="4:15">
@@ -4222,7 +4285,7 @@
         <v>175</v>
       </c>
       <c r="O98" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="4:15">
@@ -4254,7 +4317,7 @@
         <v>175</v>
       </c>
       <c r="O99" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="4:15">
@@ -4286,7 +4349,7 @@
         <v>175</v>
       </c>
       <c r="O100" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" spans="4:15">
@@ -4318,7 +4381,7 @@
         <v>175</v>
       </c>
       <c r="O101" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="4:15">
@@ -4830,7 +4893,7 @@
         <v>182</v>
       </c>
       <c r="O117" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="118" spans="4:15">
@@ -4862,7 +4925,7 @@
         <v>183</v>
       </c>
       <c r="O118" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="119" spans="4:15">
@@ -4894,7 +4957,7 @@
         <v>184</v>
       </c>
       <c r="O119" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="120" spans="4:15">
@@ -4926,7 +4989,7 @@
         <v>185</v>
       </c>
       <c r="O120" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="121" spans="4:15">
@@ -4958,7 +5021,7 @@
         <v>169</v>
       </c>
       <c r="O121" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="122" spans="4:15">
@@ -4990,7 +5053,7 @@
         <v>186</v>
       </c>
       <c r="O122" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="123" spans="4:15">
@@ -5022,7 +5085,7 @@
         <v>169</v>
       </c>
       <c r="O123" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="124" spans="4:15">
@@ -5054,7 +5117,7 @@
         <v>187</v>
       </c>
       <c r="O124" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="125" spans="4:15">
@@ -5086,7 +5149,7 @@
         <v>188</v>
       </c>
       <c r="O125" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="126" spans="4:15">
@@ -5118,7 +5181,7 @@
         <v>189</v>
       </c>
       <c r="O126" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="127" spans="4:15">
@@ -5150,7 +5213,7 @@
         <v>169</v>
       </c>
       <c r="O127" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="128" spans="4:15">
@@ -5182,7 +5245,7 @@
         <v>190</v>
       </c>
       <c r="O128" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="129" spans="4:15">
@@ -5214,7 +5277,7 @@
         <v>191</v>
       </c>
       <c r="O129" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="130" spans="4:15">
@@ -5246,7 +5309,7 @@
         <v>169</v>
       </c>
       <c r="O130" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="131" spans="4:15">
@@ -5278,7 +5341,7 @@
         <v>169</v>
       </c>
       <c r="O131" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="132" spans="4:15">
@@ -5310,7 +5373,7 @@
         <v>169</v>
       </c>
       <c r="O132" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="133" spans="4:15">
@@ -5342,7 +5405,7 @@
         <v>169</v>
       </c>
       <c r="O133" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="134" spans="4:15">
@@ -5374,7 +5437,7 @@
         <v>192</v>
       </c>
       <c r="O134" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="135" spans="4:15">
@@ -5406,7 +5469,7 @@
         <v>193</v>
       </c>
       <c r="O135" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="136" spans="4:15">
@@ -5438,7 +5501,7 @@
         <v>194</v>
       </c>
       <c r="O136" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="4:15">
@@ -5467,7 +5530,7 @@
         <v>731835900880</v>
       </c>
       <c r="O137" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="138" spans="4:15">
@@ -5496,7 +5559,7 @@
         <v>731835900708</v>
       </c>
       <c r="O138" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="139" spans="4:15">
@@ -5525,7 +5588,7 @@
         <v>731835901003</v>
       </c>
       <c r="O139" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="140" spans="4:15">
@@ -5554,7 +5617,7 @@
         <v>731835900538</v>
       </c>
       <c r="O140" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="141" spans="4:15">
@@ -5583,7 +5646,7 @@
         <v>731835901429</v>
       </c>
       <c r="O141" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="142" spans="4:15">
@@ -5612,7 +5675,7 @@
         <v>731835901771</v>
       </c>
       <c r="O142" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="143" spans="4:15">
@@ -5641,7 +5704,7 @@
         <v>731835901933</v>
       </c>
       <c r="O143" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="144" spans="4:15">
@@ -5670,7 +5733,7 @@
         <v>731835902743</v>
       </c>
       <c r="O144" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="145" spans="4:15">
@@ -5699,7 +5762,7 @@
         <v>731835903391</v>
       </c>
       <c r="O145" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="146" spans="4:15">
@@ -5728,7 +5791,7 @@
         <v>731835902824</v>
       </c>
       <c r="O146" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="147" spans="4:15">
@@ -5757,7 +5820,7 @@
         <v>731835902310</v>
       </c>
       <c r="O147" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="148" spans="4:15">
@@ -5786,7 +5849,7 @@
         <v>731835903472</v>
       </c>
       <c r="O148" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="149" spans="4:15">
@@ -5815,7 +5878,7 @@
         <v>731835902905</v>
       </c>
       <c r="O149" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="150" spans="4:15">
@@ -5844,7 +5907,7 @@
         <v>731835903200</v>
       </c>
       <c r="O150" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="151" spans="4:15">
@@ -5873,7 +5936,7 @@
         <v>731835903049</v>
       </c>
       <c r="O151" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="152" spans="4:15">
@@ -5902,7 +5965,7 @@
         <v>731835902409</v>
       </c>
       <c r="O152" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="153" spans="4:15">
@@ -5931,7 +5994,7 @@
         <v>731835903120</v>
       </c>
       <c r="O153" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="154" spans="4:15">
@@ -5960,7 +6023,7 @@
         <v>731835903634</v>
       </c>
       <c r="O154" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="155" spans="4:15">
@@ -5989,7 +6052,7 @@
         <v>731835902581</v>
       </c>
       <c r="O155" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="156" spans="4:15">
@@ -6018,7 +6081,7 @@
         <v>731835903715</v>
       </c>
       <c r="O156" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="157" spans="4:15">
@@ -6047,7 +6110,7 @@
         <v>731835903804</v>
       </c>
       <c r="O157" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="158" spans="4:15">
@@ -6076,7 +6139,7 @@
         <v>731835902662</v>
       </c>
       <c r="O158" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="159" spans="4:15">
@@ -6105,7 +6168,7 @@
         <v>731835900104</v>
       </c>
       <c r="O159" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="160" spans="4:15">
@@ -6134,7 +6197,7 @@
         <v>731835904282</v>
       </c>
       <c r="O160" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="161" spans="4:15">
@@ -6166,7 +6229,7 @@
         <v>195</v>
       </c>
       <c r="O161" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="162" spans="4:15">
@@ -6198,7 +6261,7 @@
         <v>195</v>
       </c>
       <c r="O162" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="163" spans="4:15">
@@ -6230,7 +6293,7 @@
         <v>195</v>
       </c>
       <c r="O163" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="164" spans="4:15">
@@ -6262,7 +6325,7 @@
         <v>195</v>
       </c>
       <c r="O164" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="165" spans="4:15">
@@ -6294,7 +6357,7 @@
         <v>195</v>
       </c>
       <c r="O165" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="166" spans="4:15">
@@ -6326,7 +6389,7 @@
         <v>195</v>
       </c>
       <c r="O166" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="167" spans="4:15">
@@ -6358,7 +6421,7 @@
         <v>195</v>
       </c>
       <c r="O167" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="168" spans="4:15">
@@ -6390,7 +6453,7 @@
         <v>195</v>
       </c>
       <c r="O168" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="169" spans="4:15">
@@ -6422,7 +6485,7 @@
         <v>195</v>
       </c>
       <c r="O169" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="170" spans="4:15">
@@ -6454,7 +6517,7 @@
         <v>195</v>
       </c>
       <c r="O170" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="171" spans="4:15">
@@ -6486,7 +6549,7 @@
         <v>195</v>
       </c>
       <c r="O171" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="172" spans="4:15">
@@ -6518,7 +6581,7 @@
         <v>195</v>
       </c>
       <c r="O172" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="173" spans="4:15">
@@ -6550,7 +6613,7 @@
         <v>195</v>
       </c>
       <c r="O173" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="174" spans="4:15">
@@ -6582,7 +6645,7 @@
         <v>195</v>
       </c>
       <c r="O174" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="175" spans="4:15">
@@ -6614,7 +6677,7 @@
         <v>195</v>
       </c>
       <c r="O175" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="176" spans="4:15">
@@ -6646,7 +6709,7 @@
         <v>195</v>
       </c>
       <c r="O176" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="177" spans="4:15">
@@ -6678,7 +6741,7 @@
         <v>195</v>
       </c>
       <c r="O177" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="178" spans="4:15">
@@ -6710,7 +6773,7 @@
         <v>195</v>
       </c>
       <c r="O178" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Make captcha solving function more generic for Rio de Janeiro
</commit_message>
<xml_diff>
--- a/ValidarAcessoPrefeituras.xlsx
+++ b/ValidarAcessoPrefeituras.xlsx
@@ -1479,7 +1479,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>PÁGINA NÃO ABRIU</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2205,7 +2205,7 @@
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2256,7 +2256,7 @@
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2358,7 +2358,7 @@
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2511,7 +2511,7 @@
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2562,7 +2562,7 @@
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2664,7 +2664,7 @@
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2715,7 +2715,7 @@
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2766,7 +2766,7 @@
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2868,7 +2868,7 @@
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2919,7 +2919,7 @@
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -2970,7 +2970,7 @@
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3072,7 +3072,7 @@
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3123,7 +3123,7 @@
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3174,7 +3174,7 @@
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3225,7 +3225,7 @@
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3276,7 +3276,7 @@
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3327,7 +3327,7 @@
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3378,7 +3378,7 @@
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3429,7 +3429,7 @@
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3480,7 +3480,7 @@
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3582,7 +3582,7 @@
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3633,7 +3633,7 @@
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3684,7 +3684,7 @@
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3735,7 +3735,7 @@
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3837,7 +3837,7 @@
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3888,7 +3888,7 @@
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3939,7 +3939,7 @@
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -3990,7 +3990,7 @@
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4092,7 +4092,7 @@
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4143,7 +4143,7 @@
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4194,7 +4194,7 @@
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4296,7 +4296,7 @@
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4347,7 +4347,7 @@
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4398,7 +4398,7 @@
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4500,7 +4500,7 @@
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4551,7 +4551,7 @@
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4602,7 +4602,7 @@
       <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4653,7 +4653,7 @@
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4704,7 +4704,7 @@
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4755,7 +4755,7 @@
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4806,7 +4806,7 @@
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4908,7 +4908,7 @@
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -4959,7 +4959,7 @@
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5010,7 +5010,7 @@
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5061,7 +5061,7 @@
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5112,7 +5112,7 @@
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5163,7 +5163,7 @@
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5214,7 +5214,7 @@
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5316,7 +5316,7 @@
       <c r="N93" t="inlineStr"/>
       <c r="O93" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5418,7 +5418,7 @@
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5471,7 +5471,7 @@
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5522,7 +5522,7 @@
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5573,7 +5573,7 @@
       <c r="N98" t="inlineStr"/>
       <c r="O98" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5624,7 +5624,7 @@
       <c r="N99" t="inlineStr"/>
       <c r="O99" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5677,7 +5677,7 @@
       <c r="N100" t="inlineStr"/>
       <c r="O100" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5728,7 +5728,7 @@
       <c r="N101" t="inlineStr"/>
       <c r="O101" t="inlineStr">
         <is>
-          <t>Senha Inválida.</t>
+          <t>LOGIN VÁLIDO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Update captcha solving functionality for Guarulhos
</commit_message>
<xml_diff>
--- a/ValidarAcessoPrefeituras.xlsx
+++ b/ValidarAcessoPrefeituras.xlsx
@@ -561,11 +561,7 @@
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -614,11 +610,7 @@
         <v>33041260</v>
       </c>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>PÁGINA NÃO ABRIU</t>
-        </is>
-      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -675,11 +667,7 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -736,11 +724,7 @@
           <t>NÃO</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
-        </is>
-      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -793,11 +777,7 @@
         </is>
       </c>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>LOGIN INVALIDO</t>
-        </is>
-      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -848,11 +828,7 @@
         </is>
       </c>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -905,11 +881,7 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -962,11 +934,7 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -1019,11 +987,7 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -1076,11 +1040,7 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -1133,11 +1093,7 @@
         </is>
       </c>
       <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>PÁGINA NÃO ABRIU</t>
-        </is>
-      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -1186,11 +1142,7 @@
         <v>783856</v>
       </c>
       <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>LOGIN INVALIDO</t>
-        </is>
-      </c>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -1243,11 +1195,7 @@
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>FALTA INFORMAÇÃO</t>
-        </is>
-      </c>
+      <c r="O14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -1302,11 +1250,7 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
-        </is>
-      </c>
+      <c r="O15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
@@ -1357,11 +1301,7 @@
         </is>
       </c>
       <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
-        </is>
-      </c>
+      <c r="O16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -1414,11 +1354,7 @@
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -1477,11 +1413,7 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -1538,11 +1470,7 @@
           <t>SIM</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -1591,11 +1519,7 @@
         <v>1033</v>
       </c>
       <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
-        </is>
-      </c>
+      <c r="O20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -1642,11 +1566,7 @@
         </is>
       </c>
       <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -1693,11 +1613,7 @@
         </is>
       </c>
       <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
@@ -1744,11 +1660,7 @@
         </is>
       </c>
       <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -1795,11 +1707,7 @@
         </is>
       </c>
       <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -1846,11 +1754,7 @@
         </is>
       </c>
       <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -1897,11 +1801,7 @@
         </is>
       </c>
       <c r="N26" t="inlineStr"/>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -1948,11 +1848,7 @@
         </is>
       </c>
       <c r="N27" t="inlineStr"/>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
@@ -1999,11 +1895,7 @@
         </is>
       </c>
       <c r="N28" t="inlineStr"/>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
@@ -2050,11 +1942,7 @@
         </is>
       </c>
       <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
@@ -2101,11 +1989,7 @@
         </is>
       </c>
       <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
@@ -2152,11 +2036,7 @@
         </is>
       </c>
       <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
@@ -2203,11 +2083,7 @@
         </is>
       </c>
       <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
@@ -2254,11 +2130,7 @@
         </is>
       </c>
       <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
@@ -2305,11 +2177,7 @@
         </is>
       </c>
       <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -2356,11 +2224,7 @@
         </is>
       </c>
       <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
@@ -2407,11 +2271,7 @@
         </is>
       </c>
       <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
@@ -2458,11 +2318,7 @@
         </is>
       </c>
       <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
@@ -2509,11 +2365,7 @@
         </is>
       </c>
       <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr"/>
@@ -2560,11 +2412,7 @@
         </is>
       </c>
       <c r="N39" t="inlineStr"/>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
@@ -2611,11 +2459,7 @@
         </is>
       </c>
       <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr"/>
@@ -2662,11 +2506,7 @@
         </is>
       </c>
       <c r="N41" t="inlineStr"/>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
@@ -2713,11 +2553,7 @@
         </is>
       </c>
       <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -2764,11 +2600,7 @@
         </is>
       </c>
       <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr"/>
@@ -2815,11 +2647,7 @@
         </is>
       </c>
       <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr"/>
@@ -2866,11 +2694,7 @@
         </is>
       </c>
       <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr"/>
@@ -2917,11 +2741,7 @@
         </is>
       </c>
       <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
@@ -2968,11 +2788,7 @@
         </is>
       </c>
       <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr"/>
@@ -3019,11 +2835,7 @@
         </is>
       </c>
       <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr"/>
@@ -3070,11 +2882,7 @@
         </is>
       </c>
       <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
@@ -3121,11 +2929,7 @@
         </is>
       </c>
       <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
@@ -3172,11 +2976,7 @@
         </is>
       </c>
       <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr"/>
@@ -3223,11 +3023,7 @@
         </is>
       </c>
       <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr"/>
@@ -3274,11 +3070,7 @@
         </is>
       </c>
       <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr"/>
@@ -3325,11 +3117,7 @@
         </is>
       </c>
       <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
@@ -3376,11 +3164,7 @@
         </is>
       </c>
       <c r="N55" t="inlineStr"/>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr"/>
@@ -3427,11 +3211,7 @@
         </is>
       </c>
       <c r="N56" t="inlineStr"/>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr"/>
@@ -3478,11 +3258,7 @@
         </is>
       </c>
       <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr"/>
@@ -3529,11 +3305,7 @@
         </is>
       </c>
       <c r="N58" t="inlineStr"/>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr"/>
@@ -3580,11 +3352,7 @@
         </is>
       </c>
       <c r="N59" t="inlineStr"/>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr"/>
@@ -3631,11 +3399,7 @@
         </is>
       </c>
       <c r="N60" t="inlineStr"/>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr"/>
@@ -3682,11 +3446,7 @@
         </is>
       </c>
       <c r="N61" t="inlineStr"/>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr"/>
@@ -3733,11 +3493,7 @@
         </is>
       </c>
       <c r="N62" t="inlineStr"/>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
@@ -3784,11 +3540,7 @@
         </is>
       </c>
       <c r="N63" t="inlineStr"/>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr"/>
@@ -3835,11 +3587,7 @@
         </is>
       </c>
       <c r="N64" t="inlineStr"/>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr"/>
@@ -3886,11 +3634,7 @@
         </is>
       </c>
       <c r="N65" t="inlineStr"/>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr"/>
@@ -3937,11 +3681,7 @@
         </is>
       </c>
       <c r="N66" t="inlineStr"/>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr"/>
@@ -3988,11 +3728,7 @@
         </is>
       </c>
       <c r="N67" t="inlineStr"/>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr"/>
@@ -4039,11 +3775,7 @@
         </is>
       </c>
       <c r="N68" t="inlineStr"/>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr"/>
@@ -4090,11 +3822,7 @@
         </is>
       </c>
       <c r="N69" t="inlineStr"/>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr"/>
@@ -4141,11 +3869,7 @@
         </is>
       </c>
       <c r="N70" t="inlineStr"/>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr"/>
@@ -4192,11 +3916,7 @@
         </is>
       </c>
       <c r="N71" t="inlineStr"/>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr"/>
@@ -4243,11 +3963,7 @@
         </is>
       </c>
       <c r="N72" t="inlineStr"/>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr"/>
@@ -4294,11 +4010,7 @@
         </is>
       </c>
       <c r="N73" t="inlineStr"/>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr"/>
@@ -4345,11 +4057,7 @@
         </is>
       </c>
       <c r="N74" t="inlineStr"/>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr"/>
@@ -4396,11 +4104,7 @@
         </is>
       </c>
       <c r="N75" t="inlineStr"/>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr"/>
@@ -4447,11 +4151,7 @@
         </is>
       </c>
       <c r="N76" t="inlineStr"/>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr"/>
@@ -4498,11 +4198,7 @@
         </is>
       </c>
       <c r="N77" t="inlineStr"/>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr"/>
@@ -4549,11 +4245,7 @@
         </is>
       </c>
       <c r="N78" t="inlineStr"/>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
@@ -4600,11 +4292,7 @@
         </is>
       </c>
       <c r="N79" t="inlineStr"/>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr"/>
@@ -4651,11 +4339,7 @@
         </is>
       </c>
       <c r="N80" t="inlineStr"/>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr"/>
@@ -4702,11 +4386,7 @@
         </is>
       </c>
       <c r="N81" t="inlineStr"/>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr"/>
@@ -4753,11 +4433,7 @@
         </is>
       </c>
       <c r="N82" t="inlineStr"/>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr"/>
@@ -4804,11 +4480,7 @@
         </is>
       </c>
       <c r="N83" t="inlineStr"/>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr"/>
@@ -4855,11 +4527,7 @@
         </is>
       </c>
       <c r="N84" t="inlineStr"/>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr"/>
@@ -4906,11 +4574,7 @@
         </is>
       </c>
       <c r="N85" t="inlineStr"/>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr"/>
@@ -4957,11 +4621,7 @@
         </is>
       </c>
       <c r="N86" t="inlineStr"/>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr"/>
@@ -5008,11 +4668,7 @@
         </is>
       </c>
       <c r="N87" t="inlineStr"/>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr"/>
@@ -5059,11 +4715,7 @@
         </is>
       </c>
       <c r="N88" t="inlineStr"/>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -5110,11 +4762,7 @@
         </is>
       </c>
       <c r="N89" t="inlineStr"/>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr"/>
@@ -5161,11 +4809,7 @@
         </is>
       </c>
       <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr"/>
@@ -5212,11 +4856,7 @@
         </is>
       </c>
       <c r="N91" t="inlineStr"/>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr"/>
@@ -5263,11 +4903,7 @@
         </is>
       </c>
       <c r="N92" t="inlineStr"/>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr"/>
@@ -5314,11 +4950,7 @@
         </is>
       </c>
       <c r="N93" t="inlineStr"/>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr"/>
@@ -5365,11 +4997,7 @@
         </is>
       </c>
       <c r="N94" t="inlineStr"/>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr"/>
@@ -5416,11 +5044,7 @@
         </is>
       </c>
       <c r="N95" t="inlineStr"/>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr"/>
@@ -5469,11 +5093,7 @@
         </is>
       </c>
       <c r="N96" t="inlineStr"/>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr"/>
@@ -5520,11 +5140,7 @@
         </is>
       </c>
       <c r="N97" t="inlineStr"/>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr"/>
@@ -5571,11 +5187,7 @@
         </is>
       </c>
       <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
@@ -5622,11 +5234,7 @@
         </is>
       </c>
       <c r="N99" t="inlineStr"/>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr"/>
@@ -5675,11 +5283,7 @@
         </is>
       </c>
       <c r="N100" t="inlineStr"/>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>LOGIN VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr"/>
@@ -5781,7 +5385,7 @@
       <c r="N102" t="inlineStr"/>
       <c r="O102" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5834,7 +5438,7 @@
       <c r="N103" t="inlineStr"/>
       <c r="O103" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5887,7 +5491,7 @@
       <c r="N104" t="inlineStr"/>
       <c r="O104" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5940,7 +5544,7 @@
       <c r="N105" t="inlineStr"/>
       <c r="O105" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -5993,7 +5597,7 @@
       <c r="N106" t="inlineStr"/>
       <c r="O106" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6046,7 +5650,7 @@
       <c r="N107" t="inlineStr"/>
       <c r="O107" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6097,7 +5701,7 @@
       <c r="N108" t="inlineStr"/>
       <c r="O108" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6148,7 +5752,7 @@
       <c r="N109" t="inlineStr"/>
       <c r="O109" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6201,7 +5805,7 @@
       <c r="N110" t="inlineStr"/>
       <c r="O110" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6256,7 +5860,7 @@
       <c r="N111" t="inlineStr"/>
       <c r="O111" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6307,7 +5911,7 @@
       <c r="N112" t="inlineStr"/>
       <c r="O112" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6358,7 +5962,7 @@
       <c r="N113" t="inlineStr"/>
       <c r="O113" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6411,7 +6015,7 @@
       <c r="N114" t="inlineStr"/>
       <c r="O114" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6462,7 +6066,7 @@
       <c r="N115" t="inlineStr"/>
       <c r="O115" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6513,7 +6117,7 @@
       <c r="N116" t="inlineStr"/>
       <c r="O116" t="inlineStr">
         <is>
-          <t>VERIFICAR FORMA DE ACESSO</t>
+          <t>VÁLIDO</t>
         </is>
       </c>
     </row>
@@ -6562,11 +6166,7 @@
         </is>
       </c>
       <c r="N117" t="inlineStr"/>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr"/>
@@ -6613,11 +6213,7 @@
         </is>
       </c>
       <c r="N118" t="inlineStr"/>
-      <c r="O118" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr"/>
@@ -6664,11 +6260,7 @@
         </is>
       </c>
       <c r="N119" t="inlineStr"/>
-      <c r="O119" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr"/>
@@ -6715,11 +6307,7 @@
         </is>
       </c>
       <c r="N120" t="inlineStr"/>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr"/>
@@ -6766,11 +6354,7 @@
         </is>
       </c>
       <c r="N121" t="inlineStr"/>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr"/>
@@ -6817,11 +6401,7 @@
         </is>
       </c>
       <c r="N122" t="inlineStr"/>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr"/>
@@ -6868,11 +6448,7 @@
         </is>
       </c>
       <c r="N123" t="inlineStr"/>
-      <c r="O123" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr"/>
@@ -6919,11 +6495,7 @@
         </is>
       </c>
       <c r="N124" t="inlineStr"/>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr"/>
@@ -6970,11 +6542,7 @@
         </is>
       </c>
       <c r="N125" t="inlineStr"/>
-      <c r="O125" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr"/>
@@ -7021,11 +6589,7 @@
         </is>
       </c>
       <c r="N126" t="inlineStr"/>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr"/>
@@ -7072,11 +6636,7 @@
         </is>
       </c>
       <c r="N127" t="inlineStr"/>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr"/>
@@ -7123,11 +6683,7 @@
         </is>
       </c>
       <c r="N128" t="inlineStr"/>
-      <c r="O128" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr"/>
@@ -7174,11 +6730,7 @@
         </is>
       </c>
       <c r="N129" t="inlineStr"/>
-      <c r="O129" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr"/>
@@ -7225,11 +6777,7 @@
         </is>
       </c>
       <c r="N130" t="inlineStr"/>
-      <c r="O130" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr"/>
@@ -7276,11 +6824,7 @@
         </is>
       </c>
       <c r="N131" t="inlineStr"/>
-      <c r="O131" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr"/>
@@ -7327,11 +6871,7 @@
         </is>
       </c>
       <c r="N132" t="inlineStr"/>
-      <c r="O132" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr"/>
@@ -7378,11 +6918,7 @@
         </is>
       </c>
       <c r="N133" t="inlineStr"/>
-      <c r="O133" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr"/>
@@ -7427,11 +6963,7 @@
         </is>
       </c>
       <c r="N134" t="inlineStr"/>
-      <c r="O134" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr"/>
@@ -7476,11 +7008,7 @@
         </is>
       </c>
       <c r="N135" t="inlineStr"/>
-      <c r="O135" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr"/>
@@ -7527,11 +7055,7 @@
         </is>
       </c>
       <c r="N136" t="inlineStr"/>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>ACESSO POR CERTIFICADO</t>
-        </is>
-      </c>
+      <c r="O136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr"/>
@@ -7572,11 +7096,7 @@
       </c>
       <c r="M137" t="inlineStr"/>
       <c r="N137" t="inlineStr"/>
-      <c r="O137" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr"/>
@@ -7617,11 +7137,7 @@
       </c>
       <c r="M138" t="inlineStr"/>
       <c r="N138" t="inlineStr"/>
-      <c r="O138" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr"/>
@@ -7662,11 +7178,7 @@
       </c>
       <c r="M139" t="inlineStr"/>
       <c r="N139" t="inlineStr"/>
-      <c r="O139" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr"/>
@@ -7707,11 +7219,7 @@
       </c>
       <c r="M140" t="inlineStr"/>
       <c r="N140" t="inlineStr"/>
-      <c r="O140" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr"/>
@@ -7752,11 +7260,7 @@
       </c>
       <c r="M141" t="inlineStr"/>
       <c r="N141" t="inlineStr"/>
-      <c r="O141" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr"/>
@@ -7797,11 +7301,7 @@
       </c>
       <c r="M142" t="inlineStr"/>
       <c r="N142" t="inlineStr"/>
-      <c r="O142" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr"/>
@@ -7842,11 +7342,7 @@
       </c>
       <c r="M143" t="inlineStr"/>
       <c r="N143" t="inlineStr"/>
-      <c r="O143" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr"/>
@@ -7887,11 +7383,7 @@
       </c>
       <c r="M144" t="inlineStr"/>
       <c r="N144" t="inlineStr"/>
-      <c r="O144" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr"/>
@@ -7932,11 +7424,7 @@
       </c>
       <c r="M145" t="inlineStr"/>
       <c r="N145" t="inlineStr"/>
-      <c r="O145" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr"/>
@@ -7977,11 +7465,7 @@
       </c>
       <c r="M146" t="inlineStr"/>
       <c r="N146" t="inlineStr"/>
-      <c r="O146" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr"/>
@@ -8022,11 +7506,7 @@
       </c>
       <c r="M147" t="inlineStr"/>
       <c r="N147" t="inlineStr"/>
-      <c r="O147" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr"/>
@@ -8067,11 +7547,7 @@
       </c>
       <c r="M148" t="inlineStr"/>
       <c r="N148" t="inlineStr"/>
-      <c r="O148" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr"/>
@@ -8112,11 +7588,7 @@
       </c>
       <c r="M149" t="inlineStr"/>
       <c r="N149" t="inlineStr"/>
-      <c r="O149" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr"/>
@@ -8157,11 +7629,7 @@
       </c>
       <c r="M150" t="inlineStr"/>
       <c r="N150" t="inlineStr"/>
-      <c r="O150" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr"/>
@@ -8202,11 +7670,7 @@
       </c>
       <c r="M151" t="inlineStr"/>
       <c r="N151" t="inlineStr"/>
-      <c r="O151" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr"/>
@@ -8247,11 +7711,7 @@
       </c>
       <c r="M152" t="inlineStr"/>
       <c r="N152" t="inlineStr"/>
-      <c r="O152" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr"/>
@@ -8292,11 +7752,7 @@
       </c>
       <c r="M153" t="inlineStr"/>
       <c r="N153" t="inlineStr"/>
-      <c r="O153" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr"/>
@@ -8337,11 +7793,7 @@
       </c>
       <c r="M154" t="inlineStr"/>
       <c r="N154" t="inlineStr"/>
-      <c r="O154" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr"/>
@@ -8382,11 +7834,7 @@
       </c>
       <c r="M155" t="inlineStr"/>
       <c r="N155" t="inlineStr"/>
-      <c r="O155" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr"/>
@@ -8427,11 +7875,7 @@
       </c>
       <c r="M156" t="inlineStr"/>
       <c r="N156" t="inlineStr"/>
-      <c r="O156" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr"/>
@@ -8472,11 +7916,7 @@
       </c>
       <c r="M157" t="inlineStr"/>
       <c r="N157" t="inlineStr"/>
-      <c r="O157" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr"/>
@@ -8517,11 +7957,7 @@
       </c>
       <c r="M158" t="inlineStr"/>
       <c r="N158" t="inlineStr"/>
-      <c r="O158" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr"/>
@@ -8562,11 +7998,7 @@
       </c>
       <c r="M159" t="inlineStr"/>
       <c r="N159" t="inlineStr"/>
-      <c r="O159" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr"/>
@@ -8607,11 +8039,7 @@
       </c>
       <c r="M160" t="inlineStr"/>
       <c r="N160" t="inlineStr"/>
-      <c r="O160" t="inlineStr">
-        <is>
-          <t>Pulando</t>
-        </is>
-      </c>
+      <c r="O160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr"/>
@@ -8658,11 +8086,7 @@
         </is>
       </c>
       <c r="N161" t="inlineStr"/>
-      <c r="O161" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr"/>
@@ -8707,11 +8131,7 @@
         </is>
       </c>
       <c r="N162" t="inlineStr"/>
-      <c r="O162" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr"/>
@@ -8756,11 +8176,7 @@
         </is>
       </c>
       <c r="N163" t="inlineStr"/>
-      <c r="O163" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr"/>
@@ -8805,11 +8221,7 @@
         </is>
       </c>
       <c r="N164" t="inlineStr"/>
-      <c r="O164" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr"/>
@@ -8854,11 +8266,7 @@
         </is>
       </c>
       <c r="N165" t="inlineStr"/>
-      <c r="O165" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr"/>
@@ -8903,11 +8311,7 @@
         </is>
       </c>
       <c r="N166" t="inlineStr"/>
-      <c r="O166" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr"/>
@@ -8952,11 +8356,7 @@
         </is>
       </c>
       <c r="N167" t="inlineStr"/>
-      <c r="O167" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr"/>
@@ -9001,11 +8401,7 @@
         </is>
       </c>
       <c r="N168" t="inlineStr"/>
-      <c r="O168" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr"/>
@@ -9050,11 +8446,7 @@
         </is>
       </c>
       <c r="N169" t="inlineStr"/>
-      <c r="O169" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr"/>
@@ -9099,11 +8491,7 @@
         </is>
       </c>
       <c r="N170" t="inlineStr"/>
-      <c r="O170" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr"/>
@@ -9148,11 +8536,7 @@
         </is>
       </c>
       <c r="N171" t="inlineStr"/>
-      <c r="O171" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr"/>
@@ -9199,11 +8583,7 @@
         </is>
       </c>
       <c r="N172" t="inlineStr"/>
-      <c r="O172" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr"/>
@@ -9250,11 +8630,7 @@
         </is>
       </c>
       <c r="N173" t="inlineStr"/>
-      <c r="O173" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr"/>
@@ -9301,11 +8677,7 @@
         </is>
       </c>
       <c r="N174" t="inlineStr"/>
-      <c r="O174" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr"/>
@@ -9352,11 +8724,7 @@
         </is>
       </c>
       <c r="N175" t="inlineStr"/>
-      <c r="O175" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr"/>
@@ -9403,11 +8771,7 @@
         </is>
       </c>
       <c r="N176" t="inlineStr"/>
-      <c r="O176" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr"/>
@@ -9454,11 +8818,7 @@
         </is>
       </c>
       <c r="N177" t="inlineStr"/>
-      <c r="O177" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr"/>
@@ -9503,11 +8863,7 @@
         </is>
       </c>
       <c r="N178" t="inlineStr"/>
-      <c r="O178" t="inlineStr">
-        <is>
-          <t>VÁLIDO</t>
-        </is>
-      </c>
+      <c r="O178" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>